<commit_message>
Blends 2 cores HSV done
</commit_message>
<xml_diff>
--- a/Color Blends.xlsx
+++ b/Color Blends.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulogarcia/Desktop/MEIC/blendingbox/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PauloGarcia/Desktop/blendingbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1900" windowWidth="37380" windowHeight="22060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="87">
   <si>
     <t>Cores a Misturar</t>
   </si>
@@ -261,6 +261,30 @@
   </si>
   <si>
     <t>20 Misturas</t>
+  </si>
+  <si>
+    <t>#0000FF</t>
+  </si>
+  <si>
+    <t>#00FF80</t>
+  </si>
+  <si>
+    <t>#8000FF</t>
+  </si>
+  <si>
+    <t>#80FF00</t>
+  </si>
+  <si>
+    <t>#0080FF</t>
+  </si>
+  <si>
+    <t>#FF0080</t>
+  </si>
+  <si>
+    <t>#FF8000</t>
+  </si>
+  <si>
+    <t>#00FF00</t>
   </si>
 </sst>
 </file>
@@ -283,7 +307,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -326,8 +350,62 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8000FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF80FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0080FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0080"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -559,11 +637,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -635,55 +722,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -695,15 +743,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,14 +818,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <mruColors>
-      <color rgb="FFFFFC00"/>
-      <color rgb="FFFF0000"/>
-      <color rgb="FFFFF101"/>
-      <color rgb="FFD8117D"/>
-      <color rgb="FF00A3DB"/>
+      <color rgb="FF00FF00"/>
+      <color rgb="FF8000FF"/>
+      <color rgb="FFFF8000"/>
+      <color rgb="FFFF0080"/>
+      <color rgb="FF00FFFF"/>
+      <color rgb="FFFF00FF"/>
+      <color rgb="FFFFFF00"/>
+      <color rgb="FF0080FF"/>
+      <color rgb="FF80FF00"/>
       <color rgb="FF0000FF"/>
-      <color rgb="FF00FF00"/>
-      <color rgb="FF00FFFF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -995,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U53"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1005,10 +1113,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B2" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="46"/>
+      <c r="B2" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="33"/>
       <c r="E2" t="s">
         <v>7</v>
       </c>
@@ -1095,10 +1203,10 @@
       <c r="R8" s="20"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="27"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="11">
         <v>0</v>
       </c>
@@ -1137,10 +1245,10 @@
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="28"/>
+      <c r="C10" s="47"/>
       <c r="D10" s="11">
         <v>120</v>
       </c>
@@ -1179,10 +1287,10 @@
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="29"/>
+      <c r="C11" s="48"/>
       <c r="D11" s="11">
         <v>240</v>
       </c>
@@ -1221,10 +1329,10 @@
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="30"/>
+      <c r="C12" s="49"/>
       <c r="D12" s="11">
         <v>180</v>
       </c>
@@ -1263,10 +1371,10 @@
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="31"/>
+      <c r="C13" s="50"/>
       <c r="D13" s="11">
         <v>300</v>
       </c>
@@ -1305,10 +1413,10 @@
       </c>
     </row>
     <row r="14" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="32"/>
+      <c r="C14" s="43"/>
       <c r="D14" s="13">
         <v>60</v>
       </c>
@@ -1348,39 +1456,39 @@
     </row>
     <row r="15" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:20" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="43"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="43" t="s">
+      <c r="B16" s="36"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38" t="s">
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38" t="s">
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="K16" s="38"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="38" t="s">
+      <c r="K16" s="37"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="N16" s="38"/>
-      <c r="O16" s="38"/>
-      <c r="P16" s="38"/>
-      <c r="Q16" s="38"/>
-      <c r="R16" s="38"/>
-      <c r="S16" s="38"/>
-      <c r="T16" s="39"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="37"/>
+      <c r="Q16" s="37"/>
+      <c r="R16" s="37"/>
+      <c r="S16" s="37"/>
+      <c r="T16" s="38"/>
     </row>
     <row r="17" spans="2:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="37"/>
+      <c r="C17" s="35"/>
       <c r="D17" s="9" t="s">
         <v>39</v>
       </c>
@@ -1408,31 +1516,37 @@
       <c r="L17" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="M17" s="35" t="s">
+      <c r="M17" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="N17" s="36"/>
-      <c r="O17" s="36" t="s">
+      <c r="N17" s="41"/>
+      <c r="O17" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="P17" s="36"/>
-      <c r="Q17" s="36" t="s">
+      <c r="P17" s="41"/>
+      <c r="Q17" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="R17" s="36"/>
-      <c r="S17" s="36" t="s">
+      <c r="R17" s="41"/>
+      <c r="S17" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="T17" s="37"/>
+      <c r="T17" s="35"/>
     </row>
     <row r="18" spans="2:21" ht="17" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="48"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="11">
+        <v>60</v>
+      </c>
+      <c r="E18" s="51">
+        <v>100</v>
+      </c>
+      <c r="F18" s="51">
+        <v>100</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -1441,24 +1555,32 @@
       <c r="L18" s="12"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
+      <c r="O18" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="P18" s="59"/>
       <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
       <c r="S18" s="3"/>
       <c r="T18" s="4"/>
-      <c r="U18" s="49" t="s">
+      <c r="U18" s="28" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="48"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="27">
+        <v>300</v>
+      </c>
+      <c r="E19" s="2">
+        <v>100</v>
+      </c>
+      <c r="F19" s="2">
+        <v>100</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -1467,22 +1589,30 @@
       <c r="L19" s="12"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
+      <c r="O19" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="P19" s="60"/>
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
       <c r="S19" s="3"/>
       <c r="T19" s="4"/>
-      <c r="U19" s="49"/>
+      <c r="U19" s="28"/>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B20" s="44" t="s">
+      <c r="B20" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="45"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="27">
+        <v>180</v>
+      </c>
+      <c r="E20" s="2">
+        <v>100</v>
+      </c>
+      <c r="F20" s="2">
+        <v>100</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -1491,22 +1621,30 @@
       <c r="L20" s="12"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
+      <c r="O20" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="P20" s="61"/>
       <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
       <c r="T20" s="4"/>
-      <c r="U20" s="49"/>
+      <c r="U20" s="28"/>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="45"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="27">
+        <v>90</v>
+      </c>
+      <c r="E21" s="2">
+        <v>100</v>
+      </c>
+      <c r="F21" s="2">
+        <v>100</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -1515,22 +1653,30 @@
       <c r="L21" s="12"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
+      <c r="O21" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="P21" s="57"/>
       <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
       <c r="S21" s="3"/>
       <c r="T21" s="4"/>
-      <c r="U21" s="49"/>
+      <c r="U21" s="28"/>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B22" s="44" t="s">
+      <c r="B22" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="45"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="27">
+        <v>330</v>
+      </c>
+      <c r="E22" s="2">
+        <v>100</v>
+      </c>
+      <c r="F22" s="2">
+        <v>100</v>
+      </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -1539,22 +1685,30 @@
       <c r="L22" s="12"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
+      <c r="O22" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="P22" s="62"/>
       <c r="Q22" s="3"/>
       <c r="R22" s="3"/>
       <c r="S22" s="3"/>
       <c r="T22" s="4"/>
-      <c r="U22" s="49"/>
+      <c r="U22" s="28"/>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="27">
+        <v>30</v>
+      </c>
+      <c r="E23" s="2">
+        <v>100</v>
+      </c>
+      <c r="F23" s="2">
+        <v>100</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -1563,22 +1717,30 @@
       <c r="L23" s="12"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
+      <c r="O23" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="P23" s="63"/>
       <c r="Q23" s="3"/>
       <c r="R23" s="3"/>
       <c r="S23" s="3"/>
       <c r="T23" s="4"/>
-      <c r="U23" s="49"/>
+      <c r="U23" s="28"/>
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="45"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="27">
+        <v>240</v>
+      </c>
+      <c r="E24" s="2">
+        <v>100</v>
+      </c>
+      <c r="F24" s="2">
+        <v>100</v>
+      </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -1587,22 +1749,30 @@
       <c r="L24" s="12"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
+      <c r="O24" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="P24" s="56"/>
       <c r="Q24" s="3"/>
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
       <c r="T24" s="4"/>
-      <c r="U24" s="49"/>
+      <c r="U24" s="28"/>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="45"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="27">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2">
+        <v>100</v>
+      </c>
+      <c r="F25" s="2">
+        <v>100</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -1611,22 +1781,30 @@
       <c r="L25" s="12"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
+      <c r="O25" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="P25" s="55"/>
       <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
       <c r="S25" s="3"/>
       <c r="T25" s="4"/>
-      <c r="U25" s="49"/>
+      <c r="U25" s="28"/>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B26" s="44" t="s">
+      <c r="B26" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="45"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="27">
+        <v>150</v>
+      </c>
+      <c r="E26" s="2">
+        <v>100</v>
+      </c>
+      <c r="F26" s="2">
+        <v>100</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -1635,22 +1813,30 @@
       <c r="L26" s="12"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
+      <c r="O26" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="P26" s="54"/>
       <c r="Q26" s="3"/>
       <c r="R26" s="3"/>
       <c r="S26" s="3"/>
       <c r="T26" s="4"/>
-      <c r="U26" s="49"/>
+      <c r="U26" s="28"/>
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B27" s="44" t="s">
+      <c r="B27" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="45"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="27">
+        <v>210</v>
+      </c>
+      <c r="E27" s="2">
+        <v>100</v>
+      </c>
+      <c r="F27" s="2">
+        <v>100</v>
+      </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -1659,22 +1845,30 @@
       <c r="L27" s="12"/>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
+      <c r="O27" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="P27" s="58"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
       <c r="S27" s="3"/>
       <c r="T27" s="4"/>
-      <c r="U27" s="49"/>
+      <c r="U27" s="28"/>
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="45"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="27">
+        <v>90</v>
+      </c>
+      <c r="E28" s="2">
+        <v>100</v>
+      </c>
+      <c r="F28" s="2">
+        <v>100</v>
+      </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -1683,22 +1877,30 @@
       <c r="L28" s="12"/>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
+      <c r="O28" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="P28" s="57"/>
       <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
       <c r="S28" s="3"/>
       <c r="T28" s="4"/>
-      <c r="U28" s="49"/>
+      <c r="U28" s="28"/>
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B29" s="44" t="s">
+      <c r="B29" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="45"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="27">
+        <v>210</v>
+      </c>
+      <c r="E29" s="2">
+        <v>100</v>
+      </c>
+      <c r="F29" s="2">
+        <v>100</v>
+      </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -1707,22 +1909,30 @@
       <c r="L29" s="12"/>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
+      <c r="O29" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="P29" s="58"/>
       <c r="Q29" s="3"/>
       <c r="R29" s="3"/>
       <c r="S29" s="3"/>
       <c r="T29" s="4"/>
-      <c r="U29" s="49"/>
+      <c r="U29" s="28"/>
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B30" s="44" t="s">
+      <c r="B30" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="45"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="27">
+        <v>270</v>
+      </c>
+      <c r="E30" s="2">
+        <v>100</v>
+      </c>
+      <c r="F30" s="2">
+        <v>100</v>
+      </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -1731,22 +1941,30 @@
       <c r="L30" s="12"/>
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
+      <c r="O30" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="P30" s="53"/>
       <c r="Q30" s="3"/>
       <c r="R30" s="3"/>
       <c r="S30" s="3"/>
       <c r="T30" s="4"/>
-      <c r="U30" s="49"/>
+      <c r="U30" s="28"/>
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B31" s="44" t="s">
+      <c r="B31" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="45"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="27">
+        <v>150</v>
+      </c>
+      <c r="E31" s="2">
+        <v>100</v>
+      </c>
+      <c r="F31" s="2">
+        <v>100</v>
+      </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -1755,22 +1973,30 @@
       <c r="L31" s="12"/>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
+      <c r="O31" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="P31" s="54"/>
       <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
       <c r="S31" s="3"/>
       <c r="T31" s="4"/>
-      <c r="U31" s="49"/>
+      <c r="U31" s="28"/>
     </row>
     <row r="32" spans="2:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="44" t="s">
+      <c r="B32" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="45"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="27">
+        <v>120</v>
+      </c>
+      <c r="E32" s="2">
+        <v>100</v>
+      </c>
+      <c r="F32" s="2">
+        <v>100</v>
+      </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -1779,42 +2005,44 @@
       <c r="L32" s="12"/>
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
-      <c r="O32" s="3"/>
-      <c r="P32" s="3"/>
+      <c r="O32" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="P32" s="64"/>
       <c r="Q32" s="3"/>
       <c r="R32" s="3"/>
       <c r="S32" s="3"/>
       <c r="T32" s="4"/>
-      <c r="U32" s="49"/>
+      <c r="U32" s="28"/>
     </row>
     <row r="33" spans="2:21" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="40" t="s">
+      <c r="B33" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="42"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="41"/>
-      <c r="J33" s="41"/>
-      <c r="K33" s="41"/>
-      <c r="L33" s="42"/>
-      <c r="M33" s="41"/>
-      <c r="N33" s="41"/>
-      <c r="O33" s="41"/>
-      <c r="P33" s="41"/>
-      <c r="Q33" s="41"/>
-      <c r="R33" s="41"/>
-      <c r="S33" s="41"/>
-      <c r="T33" s="42"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="42"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="42"/>
+      <c r="H33" s="42"/>
+      <c r="I33" s="42"/>
+      <c r="J33" s="42"/>
+      <c r="K33" s="42"/>
+      <c r="L33" s="40"/>
+      <c r="M33" s="42"/>
+      <c r="N33" s="42"/>
+      <c r="O33" s="42"/>
+      <c r="P33" s="42"/>
+      <c r="Q33" s="42"/>
+      <c r="R33" s="42"/>
+      <c r="S33" s="42"/>
+      <c r="T33" s="40"/>
     </row>
     <row r="34" spans="2:21" ht="17" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="44" t="s">
+      <c r="B34" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="45"/>
+      <c r="C34" s="32"/>
       <c r="D34" s="11"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -1832,15 +2060,15 @@
       <c r="R34" s="3"/>
       <c r="S34" s="3"/>
       <c r="T34" s="4"/>
-      <c r="U34" s="49" t="s">
+      <c r="U34" s="28" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="35" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B35" s="44" t="s">
+      <c r="B35" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="45"/>
+      <c r="C35" s="32"/>
       <c r="D35" s="11"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
@@ -1858,13 +2086,13 @@
       <c r="R35" s="3"/>
       <c r="S35" s="3"/>
       <c r="T35" s="4"/>
-      <c r="U35" s="49"/>
+      <c r="U35" s="28"/>
     </row>
     <row r="36" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B36" s="44" t="s">
+      <c r="B36" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="C36" s="45"/>
+      <c r="C36" s="32"/>
       <c r="D36" s="11"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -1882,13 +2110,13 @@
       <c r="R36" s="3"/>
       <c r="S36" s="3"/>
       <c r="T36" s="4"/>
-      <c r="U36" s="49"/>
+      <c r="U36" s="28"/>
     </row>
     <row r="37" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B37" s="44" t="s">
+      <c r="B37" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="45"/>
+      <c r="C37" s="32"/>
       <c r="D37" s="11"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -1906,13 +2134,13 @@
       <c r="R37" s="3"/>
       <c r="S37" s="3"/>
       <c r="T37" s="4"/>
-      <c r="U37" s="49"/>
+      <c r="U37" s="28"/>
     </row>
     <row r="38" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B38" s="44" t="s">
+      <c r="B38" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="45"/>
+      <c r="C38" s="32"/>
       <c r="D38" s="11"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
@@ -1930,13 +2158,13 @@
       <c r="R38" s="3"/>
       <c r="S38" s="3"/>
       <c r="T38" s="4"/>
-      <c r="U38" s="49"/>
+      <c r="U38" s="28"/>
     </row>
     <row r="39" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B39" s="44" t="s">
+      <c r="B39" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="45"/>
+      <c r="C39" s="32"/>
       <c r="D39" s="11"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
@@ -1954,13 +2182,13 @@
       <c r="R39" s="3"/>
       <c r="S39" s="3"/>
       <c r="T39" s="4"/>
-      <c r="U39" s="49"/>
+      <c r="U39" s="28"/>
     </row>
     <row r="40" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B40" s="44" t="s">
+      <c r="B40" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="C40" s="45"/>
+      <c r="C40" s="32"/>
       <c r="D40" s="11"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
@@ -1978,13 +2206,13 @@
       <c r="R40" s="3"/>
       <c r="S40" s="3"/>
       <c r="T40" s="4"/>
-      <c r="U40" s="49"/>
+      <c r="U40" s="28"/>
     </row>
     <row r="41" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B41" s="44" t="s">
+      <c r="B41" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="45"/>
+      <c r="C41" s="32"/>
       <c r="D41" s="11"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
@@ -2002,13 +2230,13 @@
       <c r="R41" s="3"/>
       <c r="S41" s="3"/>
       <c r="T41" s="4"/>
-      <c r="U41" s="49"/>
+      <c r="U41" s="28"/>
     </row>
     <row r="42" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B42" s="44" t="s">
+      <c r="B42" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C42" s="45"/>
+      <c r="C42" s="32"/>
       <c r="D42" s="11"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
@@ -2026,13 +2254,13 @@
       <c r="R42" s="3"/>
       <c r="S42" s="3"/>
       <c r="T42" s="4"/>
-      <c r="U42" s="49"/>
+      <c r="U42" s="28"/>
     </row>
     <row r="43" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B43" s="44" t="s">
+      <c r="B43" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="C43" s="45"/>
+      <c r="C43" s="32"/>
       <c r="D43" s="11"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
@@ -2050,13 +2278,13 @@
       <c r="R43" s="3"/>
       <c r="S43" s="3"/>
       <c r="T43" s="4"/>
-      <c r="U43" s="49"/>
+      <c r="U43" s="28"/>
     </row>
     <row r="44" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B44" s="44" t="s">
+      <c r="B44" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="C44" s="45"/>
+      <c r="C44" s="32"/>
       <c r="D44" s="11"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
@@ -2074,13 +2302,13 @@
       <c r="R44" s="3"/>
       <c r="S44" s="3"/>
       <c r="T44" s="4"/>
-      <c r="U44" s="49"/>
+      <c r="U44" s="28"/>
     </row>
     <row r="45" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B45" s="44" t="s">
+      <c r="B45" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="45"/>
+      <c r="C45" s="32"/>
       <c r="D45" s="11"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
@@ -2098,13 +2326,13 @@
       <c r="R45" s="3"/>
       <c r="S45" s="3"/>
       <c r="T45" s="4"/>
-      <c r="U45" s="49"/>
+      <c r="U45" s="28"/>
     </row>
     <row r="46" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B46" s="44" t="s">
+      <c r="B46" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="45"/>
+      <c r="C46" s="32"/>
       <c r="D46" s="11"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
@@ -2122,13 +2350,13 @@
       <c r="R46" s="3"/>
       <c r="S46" s="3"/>
       <c r="T46" s="4"/>
-      <c r="U46" s="49"/>
+      <c r="U46" s="28"/>
     </row>
     <row r="47" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B47" s="44" t="s">
+      <c r="B47" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="45"/>
+      <c r="C47" s="32"/>
       <c r="D47" s="11"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
@@ -2146,13 +2374,13 @@
       <c r="R47" s="3"/>
       <c r="S47" s="3"/>
       <c r="T47" s="4"/>
-      <c r="U47" s="49"/>
+      <c r="U47" s="28"/>
     </row>
     <row r="48" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B48" s="44" t="s">
+      <c r="B48" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="C48" s="45"/>
+      <c r="C48" s="32"/>
       <c r="D48" s="11"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
@@ -2170,13 +2398,13 @@
       <c r="R48" s="3"/>
       <c r="S48" s="3"/>
       <c r="T48" s="4"/>
-      <c r="U48" s="49"/>
+      <c r="U48" s="28"/>
     </row>
     <row r="49" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B49" s="44" t="s">
+      <c r="B49" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="C49" s="45"/>
+      <c r="C49" s="32"/>
       <c r="D49" s="11"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
@@ -2194,13 +2422,13 @@
       <c r="R49" s="3"/>
       <c r="S49" s="3"/>
       <c r="T49" s="4"/>
-      <c r="U49" s="49"/>
+      <c r="U49" s="28"/>
     </row>
     <row r="50" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B50" s="44" t="s">
+      <c r="B50" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="C50" s="45"/>
+      <c r="C50" s="32"/>
       <c r="D50" s="11"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
@@ -2218,13 +2446,13 @@
       <c r="R50" s="3"/>
       <c r="S50" s="3"/>
       <c r="T50" s="4"/>
-      <c r="U50" s="49"/>
+      <c r="U50" s="28"/>
     </row>
     <row r="51" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B51" s="44" t="s">
+      <c r="B51" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="C51" s="45"/>
+      <c r="C51" s="32"/>
       <c r="D51" s="11"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
@@ -2242,13 +2470,13 @@
       <c r="R51" s="3"/>
       <c r="S51" s="3"/>
       <c r="T51" s="4"/>
-      <c r="U51" s="49"/>
+      <c r="U51" s="28"/>
     </row>
     <row r="52" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B52" s="44" t="s">
+      <c r="B52" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="C52" s="45"/>
+      <c r="C52" s="32"/>
       <c r="D52" s="11"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
@@ -2266,13 +2494,13 @@
       <c r="R52" s="3"/>
       <c r="S52" s="3"/>
       <c r="T52" s="4"/>
-      <c r="U52" s="49"/>
+      <c r="U52" s="28"/>
     </row>
     <row r="53" spans="2:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="33" t="s">
+      <c r="B53" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C53" s="34"/>
+      <c r="C53" s="45"/>
       <c r="D53" s="13"/>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
@@ -2290,29 +2518,23 @@
       <c r="R53" s="6"/>
       <c r="S53" s="6"/>
       <c r="T53" s="7"/>
-      <c r="U53" s="49"/>
+      <c r="U53" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="U34:U53"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="U18:U32"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
     <mergeCell ref="S17:T17"/>
     <mergeCell ref="M16:T16"/>
     <mergeCell ref="D33:T33"/>
@@ -2329,27 +2551,33 @@
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="J16:L16"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
+    <mergeCell ref="U34:U53"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="U18:U32"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B50:C50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
ColorBlends: todas as misturas de 2 calculadas e rectificadas.
</commit_message>
<xml_diff>
--- a/Color Blends.xlsx
+++ b/Color Blends.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulogarcia/Desktop/MEIC/blendingbox/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PauloGarcia/Desktop/blendingbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5260" yWindow="1240" windowWidth="39680" windowHeight="22760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="144">
   <si>
     <t>Cores a Misturar</t>
   </si>
@@ -305,12 +305,6 @@
     <t>h*</t>
   </si>
   <si>
-    <t>80.11</t>
-  </si>
-  <si>
-    <t>67.22</t>
-  </si>
-  <si>
     <t>LCh:</t>
   </si>
   <si>
@@ -323,75 +317,6 @@
     <t>H = tan-1(b/a)</t>
   </si>
   <si>
-    <t>-86.18</t>
-  </si>
-  <si>
-    <t>83.18</t>
-  </si>
-  <si>
-    <t>79.2</t>
-  </si>
-  <si>
-    <t>-107.86</t>
-  </si>
-  <si>
-    <t>-48.08</t>
-  </si>
-  <si>
-    <t>-14.14</t>
-  </si>
-  <si>
-    <t>98.25</t>
-  </si>
-  <si>
-    <t>-60.84</t>
-  </si>
-  <si>
-    <t>-21.56</t>
-  </si>
-  <si>
-    <t>94.48</t>
-  </si>
-  <si>
-    <t>#85753A</t>
-  </si>
-  <si>
-    <t>#812D54</t>
-  </si>
-  <si>
-    <t>#00656F</t>
-  </si>
-  <si>
-    <t>#857871</t>
-  </si>
-  <si>
-    <t>#D92053</t>
-  </si>
-  <si>
-    <t>#EB8B2D</t>
-  </si>
-  <si>
-    <t>#7F78AB</t>
-  </si>
-  <si>
-    <t>#EB8F73</t>
-  </si>
-  <si>
-    <t>#009E8E</t>
-  </si>
-  <si>
-    <t>#84BF41</t>
-  </si>
-  <si>
-    <t>#0067A5</t>
-  </si>
-  <si>
-    <t>#812C7C</t>
-  </si>
-  <si>
-    <t>#7CC192</t>
-  </si>
-  <si>
     <t>127.5</t>
   </si>
   <si>
@@ -431,22 +356,106 @@
     <t>CIE-L*a*b* - Hue</t>
   </si>
   <si>
-    <t>#2F2A20</t>
-  </si>
-  <si>
-    <t>#2E141F</t>
-  </si>
-  <si>
-    <t>#344448</t>
-  </si>
-  <si>
-    <t>#263205</t>
-  </si>
-  <si>
-    <t>#190803</t>
-  </si>
-  <si>
-    <t>#39342F</t>
+    <t>#c9ab00</t>
+  </si>
+  <si>
+    <t>#ca0088</t>
+  </si>
+  <si>
+    <t>#7d93a6</t>
+  </si>
+  <si>
+    <t>#dda581</t>
+  </si>
+  <si>
+    <t>#ff0087</t>
+  </si>
+  <si>
+    <t>#ffa100</t>
+  </si>
+  <si>
+    <t>#c6aeff</t>
+  </si>
+  <si>
+    <t>#ffa6a6</t>
+  </si>
+  <si>
+    <t>#46ff9c</t>
+  </si>
+  <si>
+    <t>#c9b2a2</t>
+  </si>
+  <si>
+    <t>#aeff00</t>
+  </si>
+  <si>
+    <t>#5792ff</t>
+  </si>
+  <si>
+    <t>#ab00ff</t>
+  </si>
+  <si>
+    <t>#ca8aaa</t>
+  </si>
+  <si>
+    <t>#c4ff9e</t>
+  </si>
+  <si>
+    <t>#adacac</t>
+  </si>
+  <si>
+    <t>#656565</t>
+  </si>
+  <si>
+    <t>#919191</t>
+  </si>
+  <si>
+    <t>#91c01d</t>
+  </si>
+  <si>
+    <t>#8c8788</t>
+  </si>
+  <si>
+    <t>#bcb9b5</t>
+  </si>
+  <si>
+    <t>#00caff</t>
+  </si>
+  <si>
+    <t>#ff705c</t>
+  </si>
+  <si>
+    <t>#00ffb7</t>
+  </si>
+  <si>
+    <t>#ff7f14</t>
+  </si>
+  <si>
+    <t>#b8ff15</t>
+  </si>
+  <si>
+    <t>#00acff</t>
+  </si>
+  <si>
+    <t>#a60ee2</t>
+  </si>
+  <si>
+    <t>#ff2059</t>
+  </si>
+  <si>
+    <t>#6effa3</t>
+  </si>
+  <si>
+    <t>#7f00ff</t>
+  </si>
+  <si>
+    <t>#ff8000</t>
+  </si>
+  <si>
+    <t>180º</t>
+  </si>
+  <si>
+    <t>#ff007f</t>
   </si>
 </sst>
 </file>
@@ -456,7 +465,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00;[Red]0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -471,8 +480,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="43">
+  <fills count="54">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -499,24 +514,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD8117D"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00A3DB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFF101"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF8000FF"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -571,84 +568,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF85753A"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF812D54"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00656F"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF857871"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD92053"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEB8B2D"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7F78AB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEB8F73"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF009E8E"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF84BF41"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0067A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF812C7C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7CC192"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF808000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -691,42 +610,204 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF2F2A20"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF2E141F"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF344448"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF263205"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF190803"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF39342F"/>
+        <fgColor rgb="FFC9AB00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCA0088"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7D93A6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDA581"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0087"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA100"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6AEFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA6A6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF46FF9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC9B2A2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAEFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5792FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAB00FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCA8AAA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC4FF9E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFADACAC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF656565"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF919191"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF91C01D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8C8788"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBCB9B5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00CAFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF705C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFB7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7F14"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB8FF15"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00ACFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA60EE2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF2059"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6EFFA3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7F00FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF007F"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -1094,11 +1175,95 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="182">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1208,94 +1373,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1353,73 +1479,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1432,10 +1503,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1462,11 +1545,207 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="41" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="48" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="51" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="51" borderId="37" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="51" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="51" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="51" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="51" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="51" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="51" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="52" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="49" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="53" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1475,16 +1754,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <mruColors>
-      <color rgb="FF39342F"/>
-      <color rgb="FF190803"/>
-      <color rgb="FF263205"/>
-      <color rgb="FF344448"/>
-      <color rgb="FF2E141F"/>
-      <color rgb="FF2F2A20"/>
-      <color rgb="FF80FF80"/>
-      <color rgb="FF0080FF"/>
-      <color rgb="FF80FF00"/>
-      <color rgb="FF00FF80"/>
+      <color rgb="FFFF007F"/>
+      <color rgb="FFFF8000"/>
+      <color rgb="FF7F00FF"/>
+      <color rgb="FF6EFFA3"/>
+      <color rgb="FFFF2059"/>
+      <color rgb="FFA60EE2"/>
+      <color rgb="FF00ACFF"/>
+      <color rgb="FFB8FF15"/>
+      <color rgb="FFFF7F14"/>
+      <color rgb="FF00FFB7"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1545,13 +1824,13 @@
     <xdr:from>
       <xdr:col>31</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
       <xdr:colOff>300970</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1851,22 +2130,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AI53"/>
+  <dimension ref="A2:AI56"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="12" width="10.1640625" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" customWidth="1"/>
+    <col min="21" max="21" width="5.5" customWidth="1"/>
+    <col min="23" max="23" width="5.5" customWidth="1"/>
+    <col min="25" max="25" width="5.5" customWidth="1"/>
+    <col min="27" max="27" width="5.5" customWidth="1"/>
+    <col min="29" max="29" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B2" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="99"/>
+      <c r="B2" s="82" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="82"/>
       <c r="E2" t="s">
         <v>7</v>
       </c>
@@ -1874,7 +2159,7 @@
         <v>85</v>
       </c>
       <c r="P2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="2:29" x14ac:dyDescent="0.2">
@@ -1882,9 +2167,9 @@
         <v>86</v>
       </c>
       <c r="P3" t="s">
-        <v>96</v>
-      </c>
-      <c r="S3" s="88"/>
+        <v>94</v>
+      </c>
+      <c r="S3" s="75"/>
     </row>
     <row r="4" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
@@ -1900,7 +2185,7 @@
         <v>87</v>
       </c>
       <c r="P4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.2">
@@ -1914,7 +2199,7 @@
         <v>9</v>
       </c>
       <c r="P5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="2:29" x14ac:dyDescent="0.2">
@@ -1985,10 +2270,10 @@
       </c>
     </row>
     <row r="9" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B9" s="106" t="s">
+      <c r="B9" s="110" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="106"/>
+      <c r="C9" s="110"/>
       <c r="D9" s="8">
         <v>0</v>
       </c>
@@ -1998,14 +2283,14 @@
       <c r="F9" s="9">
         <v>100</v>
       </c>
-      <c r="G9" s="73">
+      <c r="G9" s="60">
         <f t="shared" ref="G9:G14" si="0">Q9</f>
         <v>53.23</v>
       </c>
-      <c r="H9" s="73">
+      <c r="H9" s="60">
         <v>104.57</v>
       </c>
-      <c r="I9" s="74">
+      <c r="I9" s="61">
         <v>40</v>
       </c>
       <c r="J9" s="8">
@@ -2029,24 +2314,24 @@
       <c r="P9" s="9">
         <v>0</v>
       </c>
-      <c r="Q9" s="78">
+      <c r="Q9" s="65">
         <v>53.23</v>
       </c>
-      <c r="R9" s="79" t="s">
-        <v>93</v>
-      </c>
-      <c r="S9" s="80" t="s">
-        <v>94</v>
+      <c r="R9" s="66">
+        <v>80.11</v>
+      </c>
+      <c r="S9" s="67">
+        <v>67.22</v>
       </c>
       <c r="T9" s="21" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="10" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B10" s="107" t="s">
+      <c r="B10" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="107"/>
+      <c r="C10" s="111"/>
       <c r="D10" s="8">
         <v>120</v>
       </c>
@@ -2056,14 +2341,14 @@
       <c r="F10" s="9">
         <v>100</v>
       </c>
-      <c r="G10" s="73">
+      <c r="G10" s="60">
         <f t="shared" si="0"/>
         <v>87.74</v>
       </c>
-      <c r="H10" s="73">
+      <c r="H10" s="60">
         <v>119.77</v>
       </c>
-      <c r="I10" s="74">
+      <c r="I10" s="61">
         <v>136.01</v>
       </c>
       <c r="J10" s="8">
@@ -2087,24 +2372,24 @@
       <c r="P10" s="9">
         <v>0</v>
       </c>
-      <c r="Q10" s="78">
+      <c r="Q10" s="65">
         <v>87.74</v>
       </c>
-      <c r="R10" s="81" t="s">
-        <v>99</v>
-      </c>
-      <c r="S10" s="80" t="s">
-        <v>100</v>
+      <c r="R10" s="68">
+        <v>-86.18</v>
+      </c>
+      <c r="S10" s="67">
+        <v>83.18</v>
       </c>
       <c r="T10" s="21" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="11" spans="2:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="108" t="s">
+      <c r="B11" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="108"/>
+      <c r="C11" s="112"/>
       <c r="D11" s="29">
         <v>240</v>
       </c>
@@ -2114,14 +2399,14 @@
       <c r="F11" s="30">
         <v>100</v>
       </c>
-      <c r="G11" s="75">
+      <c r="G11" s="62">
         <f t="shared" si="0"/>
         <v>32.299999999999997</v>
       </c>
-      <c r="H11" s="75">
+      <c r="H11" s="62">
         <v>133.81</v>
       </c>
-      <c r="I11" s="76">
+      <c r="I11" s="63">
         <v>306.29000000000002</v>
       </c>
       <c r="J11" s="29">
@@ -2145,24 +2430,24 @@
       <c r="P11" s="30">
         <v>255</v>
       </c>
-      <c r="Q11" s="82">
+      <c r="Q11" s="69">
         <v>32.299999999999997</v>
       </c>
-      <c r="R11" s="83" t="s">
-        <v>101</v>
-      </c>
-      <c r="S11" s="84" t="s">
-        <v>102</v>
+      <c r="R11" s="70">
+        <v>79.2</v>
+      </c>
+      <c r="S11" s="71">
+        <v>-107.86</v>
       </c>
       <c r="T11" s="21" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="12" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B12" s="109" t="s">
+      <c r="B12" s="113" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="109"/>
+      <c r="C12" s="113"/>
       <c r="D12" s="8">
         <v>180</v>
       </c>
@@ -2172,14 +2457,14 @@
       <c r="F12" s="9">
         <v>100</v>
       </c>
-      <c r="G12" s="73">
+      <c r="G12" s="60">
         <f t="shared" si="0"/>
         <v>91.12</v>
       </c>
-      <c r="H12" s="73">
+      <c r="H12" s="60">
         <v>50.11</v>
       </c>
-      <c r="I12" s="74">
+      <c r="I12" s="61">
         <v>196.39</v>
       </c>
       <c r="J12" s="8">
@@ -2203,24 +2488,24 @@
       <c r="P12" s="9">
         <v>255</v>
       </c>
-      <c r="Q12" s="78">
+      <c r="Q12" s="65">
         <v>91.12</v>
       </c>
-      <c r="R12" s="81" t="s">
-        <v>103</v>
-      </c>
-      <c r="S12" s="85" t="s">
-        <v>104</v>
+      <c r="R12" s="68">
+        <v>-48.08</v>
+      </c>
+      <c r="S12" s="72">
+        <v>-14.14</v>
       </c>
       <c r="T12" s="21" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="13" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B13" s="110" t="s">
+      <c r="B13" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="110"/>
+      <c r="C13" s="114"/>
       <c r="D13" s="8">
         <v>300</v>
       </c>
@@ -2230,14 +2515,14 @@
       <c r="F13" s="9">
         <v>100</v>
       </c>
-      <c r="G13" s="73">
+      <c r="G13" s="60">
         <f t="shared" si="0"/>
         <v>60.32</v>
       </c>
-      <c r="H13" s="73">
+      <c r="H13" s="60">
         <v>115.56</v>
       </c>
-      <c r="I13" s="74">
+      <c r="I13" s="61">
         <v>328.23</v>
       </c>
       <c r="J13" s="8">
@@ -2261,24 +2546,24 @@
       <c r="P13" s="9">
         <v>255</v>
       </c>
-      <c r="Q13" s="78">
+      <c r="Q13" s="65">
         <v>60.32</v>
       </c>
-      <c r="R13" s="79" t="s">
-        <v>105</v>
-      </c>
-      <c r="S13" s="85" t="s">
-        <v>106</v>
+      <c r="R13" s="66">
+        <v>98.25</v>
+      </c>
+      <c r="S13" s="72">
+        <v>-60.84</v>
       </c>
       <c r="T13" s="21" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="14" spans="2:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="105" t="s">
+      <c r="B14" s="115" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="105"/>
+      <c r="C14" s="115"/>
       <c r="D14" s="10">
         <v>60</v>
       </c>
@@ -2288,14 +2573,14 @@
       <c r="F14" s="11">
         <v>100</v>
       </c>
-      <c r="G14" s="77">
+      <c r="G14" s="64">
         <f t="shared" si="0"/>
         <v>97.14</v>
       </c>
-      <c r="H14" s="75">
+      <c r="H14" s="62">
         <v>96.9</v>
       </c>
-      <c r="I14" s="76">
+      <c r="I14" s="63">
         <v>102.85</v>
       </c>
       <c r="J14" s="10">
@@ -2319,14 +2604,14 @@
       <c r="P14" s="11">
         <v>0</v>
       </c>
-      <c r="Q14" s="82">
+      <c r="Q14" s="69">
         <v>97.14</v>
       </c>
-      <c r="R14" s="86" t="s">
-        <v>107</v>
-      </c>
-      <c r="S14" s="87" t="s">
-        <v>108</v>
+      <c r="R14" s="73">
+        <v>-21.56</v>
+      </c>
+      <c r="S14" s="74">
+        <v>94.48</v>
       </c>
       <c r="T14" s="22" t="s">
         <v>74</v>
@@ -2334,52 +2619,52 @@
     </row>
     <row r="15" spans="2:29" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:29" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="102"/>
-      <c r="C16" s="104"/>
-      <c r="D16" s="102" t="s">
+      <c r="B16" s="90"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="103"/>
-      <c r="F16" s="104"/>
-      <c r="G16" s="103" t="s">
+      <c r="E16" s="91"/>
+      <c r="F16" s="92"/>
+      <c r="G16" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="103"/>
-      <c r="I16" s="104"/>
-      <c r="J16" s="102" t="s">
+      <c r="H16" s="91"/>
+      <c r="I16" s="92"/>
+      <c r="J16" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="K16" s="103"/>
-      <c r="L16" s="103"/>
-      <c r="M16" s="104"/>
-      <c r="N16" s="102" t="s">
+      <c r="K16" s="91"/>
+      <c r="L16" s="91"/>
+      <c r="M16" s="92"/>
+      <c r="N16" s="90" t="s">
         <v>27</v>
       </c>
-      <c r="O16" s="103"/>
-      <c r="P16" s="103"/>
-      <c r="Q16" s="121" t="s">
-        <v>132</v>
-      </c>
-      <c r="R16" s="122"/>
-      <c r="S16" s="123"/>
-      <c r="T16" s="115" t="s">
+      <c r="O16" s="91"/>
+      <c r="P16" s="91"/>
+      <c r="Q16" s="93" t="s">
+        <v>107</v>
+      </c>
+      <c r="R16" s="94"/>
+      <c r="S16" s="95"/>
+      <c r="T16" s="83" t="s">
         <v>64</v>
       </c>
-      <c r="U16" s="116"/>
-      <c r="V16" s="116"/>
-      <c r="W16" s="116"/>
-      <c r="X16" s="116"/>
-      <c r="Y16" s="116"/>
-      <c r="Z16" s="116"/>
-      <c r="AA16" s="116"/>
-      <c r="AB16" s="116"/>
-      <c r="AC16" s="117"/>
-    </row>
-    <row r="17" spans="2:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="100" t="s">
+      <c r="U16" s="84"/>
+      <c r="V16" s="84"/>
+      <c r="W16" s="84"/>
+      <c r="X16" s="84"/>
+      <c r="Y16" s="84"/>
+      <c r="Z16" s="84"/>
+      <c r="AA16" s="84"/>
+      <c r="AB16" s="84"/>
+      <c r="AC16" s="85"/>
+    </row>
+    <row r="17" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="108" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="101"/>
+      <c r="C17" s="109"/>
       <c r="D17" s="26" t="s">
         <v>37</v>
       </c>
@@ -2408,7 +2693,7 @@
         <v>42</v>
       </c>
       <c r="M17" s="27" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="N17" s="26" t="s">
         <v>66</v>
@@ -2419,41 +2704,41 @@
       <c r="P17" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="Q17" s="89" t="s">
+      <c r="Q17" s="76" t="s">
         <v>90</v>
       </c>
-      <c r="R17" s="90" t="s">
+      <c r="R17" s="77" t="s">
         <v>88</v>
       </c>
-      <c r="S17" s="91" t="s">
+      <c r="S17" s="78" t="s">
         <v>89</v>
       </c>
-      <c r="T17" s="124" t="s">
+      <c r="T17" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="U17" s="125"/>
-      <c r="V17" s="126" t="s">
-        <v>133</v>
-      </c>
-      <c r="W17" s="125"/>
-      <c r="X17" s="126" t="s">
+      <c r="U17" s="97"/>
+      <c r="V17" s="98" t="s">
+        <v>108</v>
+      </c>
+      <c r="W17" s="97"/>
+      <c r="X17" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="Y17" s="125"/>
-      <c r="Z17" s="126" t="s">
+      <c r="Y17" s="97"/>
+      <c r="Z17" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="AA17" s="125"/>
-      <c r="AB17" s="127" t="s">
-        <v>132</v>
-      </c>
-      <c r="AC17" s="128"/>
-    </row>
-    <row r="18" spans="2:35" ht="17" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="111" t="s">
+      <c r="AA17" s="97"/>
+      <c r="AB17" s="99" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC17" s="100"/>
+    </row>
+    <row r="18" spans="1:35" ht="17" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="112"/>
+      <c r="C18" s="102"/>
       <c r="D18" s="24">
         <v>60</v>
       </c>
@@ -2463,15 +2748,15 @@
       <c r="F18" s="35">
         <v>100</v>
       </c>
-      <c r="G18" s="79">
-        <f>(G10-G9) / 2</f>
-        <v>17.254999999999999</v>
-      </c>
-      <c r="H18" s="79">
-        <f>(H10-H9) / 2</f>
-        <v>7.6000000000000014</v>
-      </c>
-      <c r="I18" s="80">
+      <c r="G18" s="66">
+        <f>SUM(((G10-G9) / 2), G9)</f>
+        <v>70.484999999999999</v>
+      </c>
+      <c r="H18" s="66">
+        <f>SUM(((H10-H9) / 2),H9)</f>
+        <v>112.16999999999999</v>
+      </c>
+      <c r="I18" s="67">
         <v>88.01</v>
       </c>
       <c r="J18" s="39">
@@ -2487,42 +2772,55 @@
         <v>0</v>
       </c>
       <c r="N18" s="24" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="P18" s="2">
         <v>0</v>
       </c>
-      <c r="Q18" s="78"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="40"/>
+      <c r="Q18" s="116">
+        <f>SUM(((Q10-Q9) / 2), Q9)</f>
+        <v>70.484999999999999</v>
+      </c>
+      <c r="R18" s="81">
+        <f>SUM(((R9-R10)/2),R10)</f>
+        <v>-3.0349999999999966</v>
+      </c>
+      <c r="S18" s="41">
+        <f>SUM(((S10-S9)/2),S9)</f>
+        <v>75.2</v>
+      </c>
       <c r="T18" s="2" t="s">
         <v>74</v>
       </c>
       <c r="U18" s="43"/>
-      <c r="V18" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="W18" s="94"/>
-      <c r="X18" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="Y18" s="92"/>
+      <c r="V18" s="81" t="s">
+        <v>125</v>
+      </c>
+      <c r="W18" s="133"/>
+      <c r="X18" s="81" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y18" s="79"/>
       <c r="Z18" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA18" s="93"/>
-      <c r="AD18" s="118" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA18" s="79"/>
+      <c r="AB18" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AC18" s="118"/>
+      <c r="AD18" s="86" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B19" s="111" t="s">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="B19" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="112"/>
+      <c r="C19" s="102"/>
       <c r="D19" s="24">
         <v>300</v>
       </c>
@@ -2532,15 +2830,15 @@
       <c r="F19" s="25">
         <v>100</v>
       </c>
-      <c r="G19" s="79">
-        <f>(G9-G11) / 2</f>
-        <v>10.465</v>
-      </c>
-      <c r="H19" s="79">
-        <f>(H11-H9) /2</f>
-        <v>14.620000000000005</v>
-      </c>
-      <c r="I19" s="80">
+      <c r="G19" s="66">
+        <f>SUM(((G9-G11) / 2), G11)</f>
+        <v>42.765000000000001</v>
+      </c>
+      <c r="H19" s="66">
+        <f>SUM(((H11-H9) /2),H9)</f>
+        <v>119.19</v>
+      </c>
+      <c r="I19" s="67">
         <v>353.15</v>
       </c>
       <c r="J19" s="24">
@@ -2556,40 +2854,53 @@
         <v>0</v>
       </c>
       <c r="N19" s="24" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="O19" s="2">
         <v>0</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q19" s="78"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="40"/>
+        <v>97</v>
+      </c>
+      <c r="Q19" s="65">
+        <f>SUM(((Q9-Q11) / 2), Q11)</f>
+        <v>42.765000000000001</v>
+      </c>
+      <c r="R19" s="66">
+        <f>SUM(((R9-R11) /2),R11)</f>
+        <v>79.655000000000001</v>
+      </c>
+      <c r="S19" s="120">
+        <f>SUM(((S9-S11) /2),S11)</f>
+        <v>-20.320000000000007</v>
+      </c>
       <c r="T19" s="2" t="s">
         <v>73</v>
       </c>
       <c r="U19" s="44"/>
       <c r="V19" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="W19" s="129"/>
+        <v>126</v>
+      </c>
+      <c r="W19" s="134"/>
       <c r="X19" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y19" s="45"/>
+        <v>99</v>
+      </c>
+      <c r="Y19" s="55"/>
       <c r="Z19" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="AA19" s="67"/>
-      <c r="AD19" s="118"/>
-    </row>
-    <row r="20" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B20" s="95" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA19" s="55"/>
+      <c r="AB19" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AC19" s="119"/>
+      <c r="AD19" s="86"/>
+    </row>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="B20" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="96"/>
+      <c r="C20" s="104"/>
       <c r="D20" s="24">
         <v>180</v>
       </c>
@@ -2599,15 +2910,15 @@
       <c r="F20" s="25">
         <v>100</v>
       </c>
-      <c r="G20" s="79">
-        <f>(G10-G11)/2</f>
-        <v>27.72</v>
-      </c>
-      <c r="H20" s="79">
-        <f>(H11-H10)/2</f>
-        <v>7.0200000000000031</v>
-      </c>
-      <c r="I20" s="80">
+      <c r="G20" s="66">
+        <f>SUM(((G10-G11)/2), G11)</f>
+        <v>60.019999999999996</v>
+      </c>
+      <c r="H20" s="66">
+        <f>SUM(((H11-H10)/2),H10)</f>
+        <v>126.78999999999999</v>
+      </c>
+      <c r="I20" s="67">
         <f>I10+85.14</f>
         <v>221.14999999999998</v>
       </c>
@@ -2627,468 +2938,522 @@
         <v>0</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q20" s="78"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="40"/>
+        <v>97</v>
+      </c>
+      <c r="Q20" s="65">
+        <f>SUM(((Q10-Q11)/2), Q11)</f>
+        <v>60.019999999999996</v>
+      </c>
+      <c r="R20" s="66">
+        <f>SUM(((R11-R10)/2),R10)</f>
+        <v>-3.4900000000000091</v>
+      </c>
+      <c r="S20" s="120">
+        <f>SUM(((S10-S11)/2),S11)</f>
+        <v>-12.339999999999989</v>
+      </c>
       <c r="T20" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U20" s="46"/>
+      <c r="U20" s="45"/>
       <c r="V20" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="W20" s="130"/>
+        <v>127</v>
+      </c>
+      <c r="W20" s="135"/>
       <c r="X20" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y20" s="47"/>
+        <v>100</v>
+      </c>
+      <c r="Y20" s="56"/>
       <c r="Z20" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="AA20" s="68"/>
-      <c r="AD20" s="118"/>
-    </row>
-    <row r="21" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B21" s="95" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA20" s="56"/>
+      <c r="AB20" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC20" s="123"/>
+      <c r="AD20" s="86"/>
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A21" s="145" t="s">
+        <v>142</v>
+      </c>
+      <c r="B21" s="146" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="96"/>
-      <c r="D21" s="24">
+      <c r="C21" s="147"/>
+      <c r="D21" s="148">
         <v>90</v>
       </c>
-      <c r="E21" s="2">
-        <v>100</v>
-      </c>
-      <c r="F21" s="25">
-        <v>100</v>
-      </c>
-      <c r="G21" s="79">
-        <f>(G12-G9)/2</f>
-        <v>18.945000000000004</v>
-      </c>
-      <c r="H21" s="79">
-        <f>(H9-H12)/2</f>
-        <v>27.229999999999997</v>
-      </c>
-      <c r="I21" s="80">
+      <c r="E21" s="149">
+        <v>100</v>
+      </c>
+      <c r="F21" s="150">
+        <v>100</v>
+      </c>
+      <c r="G21" s="151">
+        <f>SUM(((G12-G9)/2),G9)</f>
+        <v>72.174999999999997</v>
+      </c>
+      <c r="H21" s="151">
+        <f>SUM(((H9-H12)/2),H12)</f>
+        <v>77.34</v>
+      </c>
+      <c r="I21" s="152">
         <f>I9+78.195</f>
         <v>118.19499999999999</v>
       </c>
-      <c r="J21" s="24">
+      <c r="J21" s="148">
         <v>50</v>
       </c>
-      <c r="K21" s="2">
+      <c r="K21" s="149">
         <v>50</v>
       </c>
-      <c r="L21" s="2">
+      <c r="L21" s="149">
         <v>50</v>
       </c>
-      <c r="M21" s="25">
-        <v>0</v>
-      </c>
-      <c r="N21" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="P21" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q21" s="78"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="40"/>
-      <c r="T21" s="17" t="s">
+      <c r="M21" s="150">
+        <v>0</v>
+      </c>
+      <c r="N21" s="148" t="s">
+        <v>97</v>
+      </c>
+      <c r="O21" s="149" t="s">
+        <v>97</v>
+      </c>
+      <c r="P21" s="149" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q21" s="153">
+        <f>SUM(((Q12-Q9)/2),Q9)</f>
+        <v>72.174999999999997</v>
+      </c>
+      <c r="R21" s="151">
+        <f>SUM(((R9-R12)/2),R12)</f>
+        <v>16.015000000000001</v>
+      </c>
+      <c r="S21" s="154">
+        <f>SUM(((S9-S12)/2),S12)</f>
+        <v>26.54</v>
+      </c>
+      <c r="T21" s="155" t="s">
         <v>80</v>
       </c>
-      <c r="U21" s="48"/>
-      <c r="V21" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="W21" s="131"/>
-      <c r="X21" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="Y21" s="49"/>
-      <c r="Z21" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="AA21" s="69"/>
-      <c r="AD21" s="118"/>
-    </row>
-    <row r="22" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B22" s="95" t="s">
+      <c r="U21" s="156"/>
+      <c r="V21" s="149" t="s">
+        <v>128</v>
+      </c>
+      <c r="W21" s="157"/>
+      <c r="X21" s="149" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y21" s="158"/>
+      <c r="Z21" s="149" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA21" s="158"/>
+      <c r="AB21" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="AC21" s="159"/>
+      <c r="AD21" s="86"/>
+    </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A22" s="145"/>
+      <c r="B22" s="160"/>
+      <c r="C22" s="161"/>
+      <c r="D22" s="162">
+        <v>270</v>
+      </c>
+      <c r="E22" s="163">
+        <v>100</v>
+      </c>
+      <c r="F22" s="164">
+        <v>100</v>
+      </c>
+      <c r="G22" s="165"/>
+      <c r="H22" s="166"/>
+      <c r="I22" s="167"/>
+      <c r="J22" s="168"/>
+      <c r="K22" s="169"/>
+      <c r="L22" s="169"/>
+      <c r="M22" s="170"/>
+      <c r="N22" s="168"/>
+      <c r="O22" s="169"/>
+      <c r="P22" s="170"/>
+      <c r="Q22" s="165"/>
+      <c r="R22" s="166"/>
+      <c r="S22" s="171"/>
+      <c r="T22" s="172" t="s">
+        <v>140</v>
+      </c>
+      <c r="U22" s="173"/>
+      <c r="V22" s="168"/>
+      <c r="W22" s="170"/>
+      <c r="X22" s="168"/>
+      <c r="Y22" s="170"/>
+      <c r="Z22" s="168"/>
+      <c r="AA22" s="170"/>
+      <c r="AB22" s="168"/>
+      <c r="AC22" s="170"/>
+      <c r="AD22" s="86"/>
+    </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="B23" s="103" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="96"/>
-      <c r="D22" s="24">
+      <c r="C23" s="104"/>
+      <c r="D23" s="24">
         <v>330</v>
       </c>
-      <c r="E22" s="2">
-        <v>100</v>
-      </c>
-      <c r="F22" s="25">
-        <v>100</v>
-      </c>
-      <c r="G22" s="79">
-        <f>(G13-G9)/2</f>
-        <v>3.5450000000000017</v>
-      </c>
-      <c r="H22" s="79">
-        <f>(H13-H9)/2</f>
-        <v>5.4950000000000045</v>
-      </c>
-      <c r="I22" s="80">
+      <c r="E23" s="2">
+        <v>100</v>
+      </c>
+      <c r="F23" s="25">
+        <v>100</v>
+      </c>
+      <c r="G23" s="66">
+        <f>SUM(((G13-G9)/2),G9)</f>
+        <v>56.774999999999999</v>
+      </c>
+      <c r="H23" s="66">
+        <f>SUM(((H13-H9)/2),H9)</f>
+        <v>110.065</v>
+      </c>
+      <c r="I23" s="67">
         <v>4.12</v>
       </c>
-      <c r="J22" s="24">
-        <v>0</v>
-      </c>
-      <c r="K22" s="2">
-        <v>100</v>
-      </c>
-      <c r="L22" s="2">
+      <c r="J23" s="24">
+        <v>0</v>
+      </c>
+      <c r="K23" s="2">
+        <v>100</v>
+      </c>
+      <c r="L23" s="2">
         <v>50</v>
       </c>
-      <c r="M22" s="25">
-        <v>0</v>
-      </c>
-      <c r="N22" s="24">
+      <c r="M23" s="25">
+        <v>0</v>
+      </c>
+      <c r="N23" s="24">
         <v>255</v>
       </c>
-      <c r="O22" s="2">
-        <v>0</v>
-      </c>
-      <c r="P22" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q22" s="78"/>
-      <c r="R22" s="2"/>
-      <c r="S22" s="40"/>
-      <c r="T22" s="17" t="s">
+      <c r="O23" s="2">
+        <v>0</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q23" s="65">
+        <f>SUM(((Q13-Q9)/2),Q9)</f>
+        <v>56.774999999999999</v>
+      </c>
+      <c r="R23" s="66">
+        <f>SUM(((R13-R9)/2),R9)</f>
+        <v>89.18</v>
+      </c>
+      <c r="S23" s="120">
+        <f>SUM(((S9-S13)/2),S13)</f>
+        <v>3.1899999999999977</v>
+      </c>
+      <c r="T23" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="U22" s="50"/>
-      <c r="V22" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="W22" s="132"/>
-      <c r="X22" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="Y22" s="51"/>
-      <c r="Z22" s="2" t="s">
+      <c r="U23" s="47"/>
+      <c r="V23" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="W23" s="136"/>
+      <c r="X23" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="AA22" s="50"/>
-      <c r="AD22" s="118"/>
-    </row>
-    <row r="23" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B23" s="95" t="s">
+      <c r="Y23" s="47"/>
+      <c r="Z23" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA23" s="47"/>
+      <c r="AB23" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC23" s="124"/>
+      <c r="AD23" s="86"/>
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="B24" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="96"/>
-      <c r="D23" s="24">
+      <c r="C24" s="104"/>
+      <c r="D24" s="24">
         <v>30</v>
       </c>
-      <c r="E23" s="2">
-        <v>100</v>
-      </c>
-      <c r="F23" s="25">
-        <v>100</v>
-      </c>
-      <c r="G23" s="79">
-        <f>(G14-G9)/2</f>
-        <v>21.955000000000002</v>
-      </c>
-      <c r="H23" s="79">
-        <f>(H9-H14)/2</f>
-        <v>3.8349999999999937</v>
-      </c>
-      <c r="I23" s="80">
+      <c r="E24" s="2">
+        <v>100</v>
+      </c>
+      <c r="F24" s="25">
+        <v>100</v>
+      </c>
+      <c r="G24" s="66">
+        <f>SUM(((G14-G9)/2),G9)</f>
+        <v>75.185000000000002</v>
+      </c>
+      <c r="H24" s="66">
+        <f>SUM(((H9-H14)/2),H14)</f>
+        <v>100.735</v>
+      </c>
+      <c r="I24" s="67">
         <f>I9+31.425</f>
         <v>71.424999999999997</v>
       </c>
-      <c r="J23" s="24">
-        <v>0</v>
-      </c>
-      <c r="K23" s="2">
+      <c r="J24" s="24">
+        <v>0</v>
+      </c>
+      <c r="K24" s="2">
         <v>50</v>
       </c>
-      <c r="L23" s="2">
-        <v>100</v>
-      </c>
-      <c r="M23" s="25">
-        <v>0</v>
-      </c>
-      <c r="N23" s="24">
+      <c r="L24" s="2">
+        <v>100</v>
+      </c>
+      <c r="M24" s="25">
+        <v>0</v>
+      </c>
+      <c r="N24" s="24">
         <v>255</v>
       </c>
-      <c r="O23" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="P23" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="78"/>
-      <c r="R23" s="2"/>
-      <c r="S23" s="40"/>
-      <c r="T23" s="17" t="s">
+      <c r="O24" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="P24" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="65">
+        <f>SUM(((Q14-Q9)/2),Q9)</f>
+        <v>75.185000000000002</v>
+      </c>
+      <c r="R24" s="66">
+        <f>SUM(((R9-R14)/2),R14)</f>
+        <v>29.275000000000002</v>
+      </c>
+      <c r="S24" s="120">
+        <f>SUM(((S9-S14)/2),S14)</f>
+        <v>80.849999999999994</v>
+      </c>
+      <c r="T24" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="U23" s="52"/>
-      <c r="V23" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="W23" s="133"/>
-      <c r="X23" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y23" s="53"/>
-      <c r="Z23" s="2" t="s">
+      <c r="U24" s="48"/>
+      <c r="V24" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="W24" s="137"/>
+      <c r="X24" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AA23" s="52"/>
-      <c r="AD23" s="118"/>
-    </row>
-    <row r="24" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B24" s="95" t="s">
+      <c r="Y24" s="48"/>
+      <c r="Z24" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA24" s="48"/>
+      <c r="AB24" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC24" s="125"/>
+      <c r="AD24" s="86"/>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="B25" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="96"/>
-      <c r="D24" s="24">
+      <c r="C25" s="104"/>
+      <c r="D25" s="24">
         <v>240</v>
       </c>
-      <c r="E24" s="2">
-        <v>100</v>
-      </c>
-      <c r="F24" s="25">
-        <v>100</v>
-      </c>
-      <c r="G24" s="79">
-        <f>(G12-G13)/2</f>
-        <v>15.400000000000002</v>
-      </c>
-      <c r="H24" s="79">
-        <f>(H13-H12)/2</f>
-        <v>32.725000000000001</v>
-      </c>
-      <c r="I24" s="80">
+      <c r="E25" s="2">
+        <v>100</v>
+      </c>
+      <c r="F25" s="25">
+        <v>100</v>
+      </c>
+      <c r="G25" s="66">
+        <f>SUM(((G12-G13)/2),G13)</f>
+        <v>75.72</v>
+      </c>
+      <c r="H25" s="66">
+        <f>SUM(((H13-H12)/2),H12)</f>
+        <v>82.835000000000008</v>
+      </c>
+      <c r="I25" s="67">
         <f>I12+65.96</f>
         <v>262.34999999999997</v>
       </c>
-      <c r="J24" s="24">
+      <c r="J25" s="24">
         <v>50</v>
-      </c>
-      <c r="K24" s="2">
-        <v>50</v>
-      </c>
-      <c r="L24" s="2">
-        <v>0</v>
-      </c>
-      <c r="M24" s="25">
-        <v>0</v>
-      </c>
-      <c r="N24" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="O24" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="P24" s="2">
-        <v>255</v>
-      </c>
-      <c r="Q24" s="78"/>
-      <c r="R24" s="2"/>
-      <c r="S24" s="40"/>
-      <c r="T24" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="U24" s="54"/>
-      <c r="V24" s="24"/>
-      <c r="W24" s="25"/>
-      <c r="X24" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="Y24" s="55"/>
-      <c r="Z24" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="AA24" s="70"/>
-      <c r="AB24" s="2"/>
-      <c r="AC24" s="4"/>
-      <c r="AD24" s="118"/>
-    </row>
-    <row r="25" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B25" s="95" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="96"/>
-      <c r="D25" s="24">
-        <v>0</v>
-      </c>
-      <c r="E25" s="2">
-        <v>100</v>
-      </c>
-      <c r="F25" s="25">
-        <v>100</v>
-      </c>
-      <c r="G25" s="79">
-        <f>(G14-G13)/2</f>
-        <v>18.41</v>
-      </c>
-      <c r="H25" s="79">
-        <f>(H13-H14)/2</f>
-        <v>9.3299999999999983</v>
-      </c>
-      <c r="I25" s="80">
-        <v>35.54</v>
-      </c>
-      <c r="J25" s="24">
-        <v>0</v>
       </c>
       <c r="K25" s="2">
         <v>50</v>
       </c>
       <c r="L25" s="2">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="M25" s="25">
         <v>0</v>
       </c>
-      <c r="N25" s="24">
+      <c r="N25" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="P25" s="2">
         <v>255</v>
       </c>
-      <c r="O25" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="P25" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q25" s="78"/>
-      <c r="R25" s="2"/>
-      <c r="S25" s="40"/>
+      <c r="Q25" s="65">
+        <f>SUM(((Q12-Q13)/2),Q13)</f>
+        <v>75.72</v>
+      </c>
+      <c r="R25" s="66">
+        <f>SUM(((R13-R12)/2),R12)</f>
+        <v>25.084999999999994</v>
+      </c>
+      <c r="S25" s="120">
+        <f>SUM(((S12-S13)/2),S13)</f>
+        <v>-37.49</v>
+      </c>
       <c r="T25" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="U25" s="56"/>
-      <c r="V25" s="24"/>
-      <c r="W25" s="25"/>
-      <c r="X25" s="17" t="s">
-        <v>116</v>
+        <v>77</v>
+      </c>
+      <c r="U25" s="49"/>
+      <c r="V25" s="80" t="s">
+        <v>131</v>
+      </c>
+      <c r="W25" s="138"/>
+      <c r="X25" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="Y25" s="57"/>
       <c r="Z25" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="AA25" s="71"/>
-      <c r="AB25" s="2"/>
-      <c r="AC25" s="4"/>
-      <c r="AD25" s="118"/>
-    </row>
-    <row r="26" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B26" s="95" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA25" s="57"/>
+      <c r="AB25" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC25" s="126"/>
+      <c r="AD25" s="86"/>
+    </row>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="B26" s="103" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="104"/>
+      <c r="D26" s="24">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2">
+        <v>100</v>
+      </c>
+      <c r="F26" s="25">
+        <v>100</v>
+      </c>
+      <c r="G26" s="66">
+        <f>SUM(((G14-G13)/2),G13)</f>
+        <v>78.73</v>
+      </c>
+      <c r="H26" s="66">
+        <f>SUM(((H13-H14)/2),H14)</f>
+        <v>106.23</v>
+      </c>
+      <c r="I26" s="67">
+        <v>35.54</v>
+      </c>
+      <c r="J26" s="24">
+        <v>0</v>
+      </c>
+      <c r="K26" s="2">
+        <v>50</v>
+      </c>
+      <c r="L26" s="2">
+        <v>50</v>
+      </c>
+      <c r="M26" s="25">
+        <v>0</v>
+      </c>
+      <c r="N26" s="24">
+        <v>255</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q26" s="65">
+        <f>SUM(((Q14-Q13)/2),Q13)</f>
+        <v>78.73</v>
+      </c>
+      <c r="R26" s="66">
+        <f>SUM(((R13-R14)/2),R14)</f>
+        <v>38.344999999999999</v>
+      </c>
+      <c r="S26" s="120">
+        <f>SUM(((S14-S13)/2),S13)</f>
+        <v>16.819999999999993</v>
+      </c>
+      <c r="T26" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="U26" s="50"/>
+      <c r="V26" s="80" t="s">
+        <v>132</v>
+      </c>
+      <c r="W26" s="139"/>
+      <c r="X26" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y26" s="58"/>
+      <c r="Z26" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA26" s="58"/>
+      <c r="AB26" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC26" s="127"/>
+      <c r="AD26" s="86"/>
+    </row>
+    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="B27" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="96"/>
-      <c r="D26" s="24">
+      <c r="C27" s="104"/>
+      <c r="D27" s="24">
         <v>150</v>
       </c>
-      <c r="E26" s="2">
-        <v>100</v>
-      </c>
-      <c r="F26" s="25">
-        <v>100</v>
-      </c>
-      <c r="G26" s="79">
-        <f>(G12-G10)/2</f>
-        <v>1.6900000000000048</v>
-      </c>
-      <c r="H26" s="79">
-        <f>(H10-H12)/2</f>
-        <v>34.83</v>
-      </c>
-      <c r="I26" s="80">
+      <c r="E27" s="2">
+        <v>100</v>
+      </c>
+      <c r="F27" s="25">
+        <v>100</v>
+      </c>
+      <c r="G27" s="66">
+        <f>SUM(((G12-G10)/2),G10)</f>
+        <v>89.43</v>
+      </c>
+      <c r="H27" s="66">
+        <f>SUM(((H10-H12)/2),H12)</f>
+        <v>84.94</v>
+      </c>
+      <c r="I27" s="67">
         <f>I10+30.19</f>
         <v>166.2</v>
       </c>
-      <c r="J26" s="24">
-        <v>100</v>
-      </c>
-      <c r="K26" s="2">
-        <v>0</v>
-      </c>
-      <c r="L26" s="2">
-        <v>50</v>
-      </c>
-      <c r="M26" s="25">
-        <v>0</v>
-      </c>
-      <c r="N26" s="24">
-        <v>0</v>
-      </c>
-      <c r="O26" s="2">
-        <v>255</v>
-      </c>
-      <c r="P26" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q26" s="78"/>
-      <c r="R26" s="2"/>
-      <c r="S26" s="40"/>
-      <c r="T26" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="U26" s="58"/>
-      <c r="V26" s="24"/>
-      <c r="W26" s="25"/>
-      <c r="X26" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y26" s="59"/>
-      <c r="Z26" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA26" s="58"/>
-      <c r="AB26" s="2"/>
-      <c r="AC26" s="4"/>
-      <c r="AD26" s="118"/>
-    </row>
-    <row r="27" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B27" s="95" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="96"/>
-      <c r="D27" s="24">
-        <v>210</v>
-      </c>
-      <c r="E27" s="2">
-        <v>100</v>
-      </c>
-      <c r="F27" s="25">
-        <v>100</v>
-      </c>
-      <c r="G27" s="79">
-        <f>(G10-G13)/2</f>
-        <v>13.709999999999997</v>
-      </c>
-      <c r="H27" s="79">
-        <f>(H10-H13)/2</f>
-        <v>2.1049999999999969</v>
-      </c>
-      <c r="I27" s="80">
-        <v>52.12</v>
-      </c>
       <c r="J27" s="24">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="K27" s="2">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="L27" s="2">
         <v>50</v>
@@ -3096,551 +3461,696 @@
       <c r="M27" s="25">
         <v>0</v>
       </c>
-      <c r="N27" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="O27" s="2" t="s">
-        <v>122</v>
+      <c r="N27" s="24">
+        <v>0</v>
+      </c>
+      <c r="O27" s="2">
+        <v>255</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q27" s="78"/>
-      <c r="R27" s="2"/>
-      <c r="S27" s="40"/>
-      <c r="T27" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q27" s="65">
+        <f>SUM(((Q12-Q10)/2),Q10)</f>
+        <v>89.43</v>
+      </c>
+      <c r="R27" s="66">
+        <f>SUM(((R12-R10)/2),R10)</f>
+        <v>-67.13</v>
+      </c>
+      <c r="S27" s="120">
+        <f>SUM(((S10-S12)/2),S12)</f>
+        <v>34.520000000000003</v>
+      </c>
+      <c r="T27" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="U27" s="51"/>
+      <c r="V27" s="80" t="s">
+        <v>133</v>
+      </c>
+      <c r="W27" s="140"/>
+      <c r="X27" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y27" s="51"/>
+      <c r="Z27" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA27" s="51"/>
+      <c r="AB27" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AC27" s="128"/>
+      <c r="AD27" s="86"/>
+    </row>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A28" s="145" t="s">
+        <v>142</v>
+      </c>
+      <c r="B28" s="146" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="147"/>
+      <c r="D28" s="148">
+        <v>210</v>
+      </c>
+      <c r="E28" s="149">
+        <v>100</v>
+      </c>
+      <c r="F28" s="150">
+        <v>100</v>
+      </c>
+      <c r="G28" s="151">
+        <f>SUM(((G10-G13)/2),G13)</f>
+        <v>74.03</v>
+      </c>
+      <c r="H28" s="151">
+        <f>SUM(((H10-H13)/2),H13)</f>
+        <v>117.66499999999999</v>
+      </c>
+      <c r="I28" s="152">
+        <v>52.12</v>
+      </c>
+      <c r="J28" s="148">
+        <v>50</v>
+      </c>
+      <c r="K28" s="149">
+        <v>50</v>
+      </c>
+      <c r="L28" s="149">
+        <v>50</v>
+      </c>
+      <c r="M28" s="150">
+        <v>0</v>
+      </c>
+      <c r="N28" s="148" t="s">
+        <v>97</v>
+      </c>
+      <c r="O28" s="149" t="s">
+        <v>97</v>
+      </c>
+      <c r="P28" s="149" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q28" s="153">
+        <f>SUM(((Q10-Q13)/2),Q13)</f>
+        <v>74.03</v>
+      </c>
+      <c r="R28" s="151">
+        <f>SUM(((R13-R10)/2),R10)</f>
+        <v>6.0349999999999966</v>
+      </c>
+      <c r="S28" s="154">
+        <f>SUM(((S10-S13)/2),S13)</f>
+        <v>11.170000000000002</v>
+      </c>
+      <c r="T28" s="155" t="s">
         <v>81</v>
       </c>
-      <c r="U27" s="60"/>
-      <c r="V27" s="24"/>
-      <c r="W27" s="25"/>
-      <c r="X27" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="Y27" s="49"/>
-      <c r="Z27" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="AA27" s="69"/>
-      <c r="AB27" s="2"/>
-      <c r="AC27" s="4"/>
-      <c r="AD27" s="118"/>
-    </row>
-    <row r="28" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B28" s="95" t="s">
+      <c r="U28" s="174"/>
+      <c r="V28" s="148" t="s">
+        <v>134</v>
+      </c>
+      <c r="W28" s="175"/>
+      <c r="X28" s="149" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y28" s="158"/>
+      <c r="Z28" s="149" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA28" s="158"/>
+      <c r="AB28" s="149" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC28" s="176"/>
+      <c r="AD28" s="86"/>
+    </row>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A29" s="145"/>
+      <c r="B29" s="160"/>
+      <c r="C29" s="161"/>
+      <c r="D29" s="162">
+        <v>30</v>
+      </c>
+      <c r="E29" s="163">
+        <v>100</v>
+      </c>
+      <c r="F29" s="164">
+        <v>100</v>
+      </c>
+      <c r="G29" s="165"/>
+      <c r="H29" s="166"/>
+      <c r="I29" s="167"/>
+      <c r="J29" s="168"/>
+      <c r="K29" s="169"/>
+      <c r="L29" s="169"/>
+      <c r="M29" s="170"/>
+      <c r="N29" s="168"/>
+      <c r="O29" s="169"/>
+      <c r="P29" s="170"/>
+      <c r="Q29" s="165"/>
+      <c r="R29" s="166"/>
+      <c r="S29" s="171"/>
+      <c r="T29" s="172" t="s">
+        <v>141</v>
+      </c>
+      <c r="U29" s="177"/>
+      <c r="V29" s="168"/>
+      <c r="W29" s="170"/>
+      <c r="X29" s="168"/>
+      <c r="Y29" s="170"/>
+      <c r="Z29" s="168"/>
+      <c r="AA29" s="170"/>
+      <c r="AB29" s="168"/>
+      <c r="AC29" s="170"/>
+      <c r="AD29" s="86"/>
+    </row>
+    <row r="30" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="B30" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="96"/>
-      <c r="D28" s="24">
+      <c r="C30" s="104"/>
+      <c r="D30" s="24">
         <v>90</v>
       </c>
-      <c r="E28" s="2">
-        <v>100</v>
-      </c>
-      <c r="F28" s="25">
-        <v>100</v>
-      </c>
-      <c r="G28" s="79">
-        <f>(G14-G10)/2</f>
-        <v>4.7000000000000028</v>
-      </c>
-      <c r="H28" s="79">
-        <f>(H10-H14)/2</f>
-        <v>11.434999999999995</v>
-      </c>
-      <c r="I28" s="80">
+      <c r="E30" s="2">
+        <v>100</v>
+      </c>
+      <c r="F30" s="25">
+        <v>100</v>
+      </c>
+      <c r="G30" s="66">
+        <f>SUM(((G14-G10)/2),G10)</f>
+        <v>92.44</v>
+      </c>
+      <c r="H30" s="66">
+        <f>SUM(((H10-H14)/2),H14)</f>
+        <v>108.33500000000001</v>
+      </c>
+      <c r="I30" s="67">
         <f>I14+16.58</f>
         <v>119.42999999999999</v>
       </c>
-      <c r="J28" s="24">
+      <c r="J30" s="24">
         <v>50</v>
       </c>
-      <c r="K28" s="2">
-        <v>0</v>
-      </c>
-      <c r="L28" s="2">
-        <v>100</v>
-      </c>
-      <c r="M28" s="25">
-        <v>0</v>
-      </c>
-      <c r="N28" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="O28" s="2">
+      <c r="K30" s="2">
+        <v>0</v>
+      </c>
+      <c r="L30" s="2">
+        <v>100</v>
+      </c>
+      <c r="M30" s="25">
+        <v>0</v>
+      </c>
+      <c r="N30" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="O30" s="2">
         <v>255</v>
       </c>
-      <c r="P28" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="78"/>
-      <c r="R28" s="2"/>
-      <c r="S28" s="40"/>
-      <c r="T28" s="17" t="s">
+      <c r="P30" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="65">
+        <f>SUM(((Q14-Q10)/2),Q10)</f>
+        <v>92.44</v>
+      </c>
+      <c r="R30" s="66">
+        <f>SUM(((R14-R10)/2),R10)</f>
+        <v>-53.870000000000005</v>
+      </c>
+      <c r="S30" s="120">
+        <f>SUM(((S14-S10)/2),S10)</f>
+        <v>88.830000000000013</v>
+      </c>
+      <c r="T30" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="U28" s="48"/>
-      <c r="V28" s="24"/>
-      <c r="W28" s="25"/>
-      <c r="X28" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="Y28" s="61"/>
-      <c r="Z28" s="2" t="s">
+      <c r="U30" s="46"/>
+      <c r="V30" s="80" t="s">
+        <v>135</v>
+      </c>
+      <c r="W30" s="141"/>
+      <c r="X30" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AA28" s="48"/>
-      <c r="AB28" s="2"/>
-      <c r="AC28" s="4"/>
-      <c r="AD28" s="118"/>
-      <c r="AH28" s="99" t="s">
-        <v>134</v>
-      </c>
-      <c r="AI28" s="99"/>
-    </row>
-    <row r="29" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B29" s="95" t="s">
+      <c r="Y30" s="46"/>
+      <c r="Z30" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA30" s="46"/>
+      <c r="AB30" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC30" s="129"/>
+      <c r="AD30" s="86"/>
+      <c r="AH30" s="82" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI30" s="82"/>
+    </row>
+    <row r="31" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="B31" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="96"/>
-      <c r="D29" s="24">
+      <c r="C31" s="104"/>
+      <c r="D31" s="24">
         <v>210</v>
       </c>
-      <c r="E29" s="2">
-        <v>100</v>
-      </c>
-      <c r="F29" s="25">
-        <v>100</v>
-      </c>
-      <c r="G29" s="79">
-        <f>(G12-G11)/2</f>
-        <v>29.410000000000004</v>
-      </c>
-      <c r="H29" s="79">
-        <f>(H11-H12)/2</f>
-        <v>41.85</v>
-      </c>
-      <c r="I29" s="80">
+      <c r="E31" s="2">
+        <v>100</v>
+      </c>
+      <c r="F31" s="25">
+        <v>100</v>
+      </c>
+      <c r="G31" s="66">
+        <f>SUM(((G12-G11)/2),G11)</f>
+        <v>61.71</v>
+      </c>
+      <c r="H31" s="66">
+        <f>SUM(((H11-H12)/2),H12)</f>
+        <v>91.960000000000008</v>
+      </c>
+      <c r="I31" s="67">
         <f>I12+54.95</f>
         <v>251.33999999999997</v>
       </c>
-      <c r="J29" s="24">
-        <v>100</v>
-      </c>
-      <c r="K29" s="2">
+      <c r="J31" s="24">
+        <v>100</v>
+      </c>
+      <c r="K31" s="2">
         <v>50</v>
       </c>
-      <c r="L29" s="2">
-        <v>0</v>
-      </c>
-      <c r="M29" s="25">
-        <v>0</v>
-      </c>
-      <c r="N29" s="24">
-        <v>0</v>
-      </c>
-      <c r="O29" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="P29" s="2">
+      <c r="L31" s="2">
+        <v>0</v>
+      </c>
+      <c r="M31" s="25">
+        <v>0</v>
+      </c>
+      <c r="N31" s="24">
+        <v>0</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="P31" s="2">
         <v>255</v>
       </c>
-      <c r="Q29" s="78"/>
-      <c r="R29" s="2"/>
-      <c r="S29" s="40"/>
-      <c r="T29" s="17" t="s">
+      <c r="Q31" s="65">
+        <f>SUM(((Q12-Q11)/2),Q11)</f>
+        <v>61.71</v>
+      </c>
+      <c r="R31" s="66">
+        <f>SUM(((R11-R12)/2),R12)</f>
+        <v>15.560000000000002</v>
+      </c>
+      <c r="S31" s="120">
+        <f>SUM(((S12-S11)/2),S11)</f>
+        <v>-61</v>
+      </c>
+      <c r="T31" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="U29" s="60"/>
-      <c r="V29" s="24"/>
-      <c r="W29" s="25"/>
-      <c r="X29" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y29" s="62"/>
-      <c r="Z29" s="2" t="s">
+      <c r="U31" s="52"/>
+      <c r="V31" s="80" t="s">
+        <v>136</v>
+      </c>
+      <c r="W31" s="142"/>
+      <c r="X31" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="AA29" s="60"/>
-      <c r="AB29" s="2"/>
-      <c r="AC29" s="4"/>
-      <c r="AD29" s="118"/>
-    </row>
-    <row r="30" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B30" s="95" t="s">
+      <c r="Y31" s="52"/>
+      <c r="Z31" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA31" s="52"/>
+      <c r="AB31" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="AC31" s="130"/>
+      <c r="AD31" s="86"/>
+    </row>
+    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="B32" s="103" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="96"/>
-      <c r="D30" s="24">
+      <c r="C32" s="104"/>
+      <c r="D32" s="24">
         <v>270</v>
       </c>
-      <c r="E30" s="2">
-        <v>100</v>
-      </c>
-      <c r="F30" s="25">
-        <v>100</v>
-      </c>
-      <c r="G30" s="79">
-        <f>(G13-G11)/2</f>
-        <v>14.010000000000002</v>
-      </c>
-      <c r="H30" s="79">
-        <f>(H11-H13)/2</f>
-        <v>9.125</v>
-      </c>
-      <c r="I30" s="80">
+      <c r="E32" s="2">
+        <v>100</v>
+      </c>
+      <c r="F32" s="25">
+        <v>100</v>
+      </c>
+      <c r="G32" s="66">
+        <f>SUM(((G13-G11)/2),G11)</f>
+        <v>46.31</v>
+      </c>
+      <c r="H32" s="66">
+        <f>SUM(((H11-H13)/2),H13)</f>
+        <v>124.685</v>
+      </c>
+      <c r="I32" s="67">
         <f>I11+10.97</f>
         <v>317.26000000000005</v>
       </c>
-      <c r="J30" s="24">
+      <c r="J32" s="24">
         <v>50</v>
       </c>
-      <c r="K30" s="2">
-        <v>100</v>
-      </c>
-      <c r="L30" s="2">
-        <v>0</v>
-      </c>
-      <c r="M30" s="25">
-        <v>0</v>
-      </c>
-      <c r="N30" s="24" t="s">
+      <c r="K32" s="2">
+        <v>100</v>
+      </c>
+      <c r="L32" s="2">
+        <v>0</v>
+      </c>
+      <c r="M32" s="25">
+        <v>0</v>
+      </c>
+      <c r="N32" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="O32" s="2">
+        <v>0</v>
+      </c>
+      <c r="P32" s="2">
+        <v>255</v>
+      </c>
+      <c r="Q32" s="65">
+        <f>SUM(((Q13-Q11)/2),Q11)</f>
+        <v>46.31</v>
+      </c>
+      <c r="R32" s="66">
+        <f>SUM(((R13-R11)/2),R11)</f>
+        <v>88.724999999999994</v>
+      </c>
+      <c r="S32" s="120">
+        <f>SUM(((S13-S11)/2),S11)</f>
+        <v>-84.35</v>
+      </c>
+      <c r="T32" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="U32" s="53"/>
+      <c r="V32" s="80" t="s">
+        <v>137</v>
+      </c>
+      <c r="W32" s="143"/>
+      <c r="X32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y32" s="53"/>
+      <c r="Z32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA32" s="53"/>
+      <c r="AB32" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="O30" s="2">
-        <v>0</v>
-      </c>
-      <c r="P30" s="2">
-        <v>255</v>
-      </c>
-      <c r="Q30" s="78"/>
-      <c r="R30" s="2"/>
-      <c r="S30" s="40"/>
-      <c r="T30" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="U30" s="63"/>
-      <c r="V30" s="24"/>
-      <c r="W30" s="25"/>
-      <c r="X30" s="17" t="s">
+      <c r="AC32" s="131"/>
+      <c r="AD32" s="86"/>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A33" s="145" t="s">
+        <v>142</v>
+      </c>
+      <c r="B33" s="146" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="147"/>
+      <c r="D33" s="148">
+        <v>150</v>
+      </c>
+      <c r="E33" s="149">
+        <v>100</v>
+      </c>
+      <c r="F33" s="150">
+        <v>100</v>
+      </c>
+      <c r="G33" s="151">
+        <f>SUM(((G14-G11)/2),G11)</f>
+        <v>64.72</v>
+      </c>
+      <c r="H33" s="151">
+        <f>SUM(((H11-H14)/2),H14)</f>
+        <v>115.355</v>
+      </c>
+      <c r="I33" s="152">
+        <v>24.57</v>
+      </c>
+      <c r="J33" s="148">
+        <v>50</v>
+      </c>
+      <c r="K33" s="149">
+        <v>50</v>
+      </c>
+      <c r="L33" s="149">
+        <v>50</v>
+      </c>
+      <c r="M33" s="150">
+        <v>0</v>
+      </c>
+      <c r="N33" s="148" t="s">
+        <v>97</v>
+      </c>
+      <c r="O33" s="149" t="s">
+        <v>97</v>
+      </c>
+      <c r="P33" s="149" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q33" s="153">
+        <f>SUM(((Q14-Q11)/2),Q11)</f>
+        <v>64.72</v>
+      </c>
+      <c r="R33" s="151">
+        <f>SUM(((R11-R14)/2),R14)</f>
+        <v>28.820000000000004</v>
+      </c>
+      <c r="S33" s="154">
+        <f>SUM(((S14-S11)/2),S11)</f>
+        <v>-6.6899999999999977</v>
+      </c>
+      <c r="T33" s="149" t="s">
+        <v>78</v>
+      </c>
+      <c r="U33" s="178"/>
+      <c r="V33" s="148" t="s">
+        <v>138</v>
+      </c>
+      <c r="W33" s="179"/>
+      <c r="X33" s="149" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y33" s="158"/>
+      <c r="Z33" s="149" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA33" s="158"/>
+      <c r="AB33" s="149" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC33" s="180"/>
+      <c r="AD33" s="86"/>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A34" s="145"/>
+      <c r="B34" s="160"/>
+      <c r="C34" s="161"/>
+      <c r="D34" s="162">
+        <v>330</v>
+      </c>
+      <c r="E34" s="163">
+        <v>100</v>
+      </c>
+      <c r="F34" s="164">
+        <v>100</v>
+      </c>
+      <c r="G34" s="165"/>
+      <c r="H34" s="166"/>
+      <c r="I34" s="167"/>
+      <c r="J34" s="168"/>
+      <c r="K34" s="169"/>
+      <c r="L34" s="169"/>
+      <c r="M34" s="170"/>
+      <c r="N34" s="168"/>
+      <c r="O34" s="169"/>
+      <c r="P34" s="170"/>
+      <c r="Q34" s="165"/>
+      <c r="R34" s="166"/>
+      <c r="S34" s="171"/>
+      <c r="T34" s="172" t="s">
+        <v>143</v>
+      </c>
+      <c r="U34" s="181"/>
+      <c r="V34" s="168"/>
+      <c r="W34" s="170"/>
+      <c r="X34" s="168"/>
+      <c r="Y34" s="170"/>
+      <c r="Z34" s="168"/>
+      <c r="AA34" s="170"/>
+      <c r="AB34" s="168"/>
+      <c r="AC34" s="170"/>
+      <c r="AD34" s="86"/>
+    </row>
+    <row r="35" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="103" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="104"/>
+      <c r="D35" s="24">
         <v>120</v>
       </c>
-      <c r="Y30" s="64"/>
-      <c r="Z30" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA30" s="63"/>
-      <c r="AB30" s="2"/>
-      <c r="AC30" s="4"/>
-      <c r="AD30" s="118"/>
-    </row>
-    <row r="31" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B31" s="95" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="96"/>
-      <c r="D31" s="24">
-        <v>150</v>
-      </c>
-      <c r="E31" s="2">
-        <v>100</v>
-      </c>
-      <c r="F31" s="25">
-        <v>100</v>
-      </c>
-      <c r="G31" s="79">
-        <f>(G14-G11)/2</f>
-        <v>32.42</v>
-      </c>
-      <c r="H31" s="79">
-        <f>(H11-H14)/2</f>
-        <v>18.454999999999998</v>
-      </c>
-      <c r="I31" s="80">
-        <v>24.57</v>
-      </c>
-      <c r="J31" s="24">
-        <v>50</v>
-      </c>
-      <c r="K31" s="2">
-        <v>50</v>
-      </c>
-      <c r="L31" s="2">
-        <v>50</v>
-      </c>
-      <c r="M31" s="25">
-        <v>0</v>
-      </c>
-      <c r="N31" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="O31" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="P31" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q31" s="78"/>
-      <c r="R31" s="2"/>
-      <c r="S31" s="40"/>
-      <c r="T31" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="U31" s="58"/>
-      <c r="V31" s="24"/>
-      <c r="W31" s="25"/>
-      <c r="X31" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="Y31" s="49"/>
-      <c r="Z31" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="AA31" s="69"/>
-      <c r="AB31" s="2"/>
-      <c r="AC31" s="4"/>
-      <c r="AD31" s="118"/>
-    </row>
-    <row r="32" spans="2:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="95" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="96"/>
-      <c r="D32" s="24">
-        <v>120</v>
-      </c>
-      <c r="E32" s="2">
-        <v>100</v>
-      </c>
-      <c r="F32" s="25">
-        <v>100</v>
-      </c>
-      <c r="G32" s="79">
-        <f>(G14-G12)/2</f>
-        <v>3.009999999999998</v>
-      </c>
-      <c r="H32" s="79">
-        <f>(H14-H12)/2</f>
-        <v>23.395000000000003</v>
-      </c>
-      <c r="I32" s="80">
+      <c r="E35" s="2">
+        <v>100</v>
+      </c>
+      <c r="F35" s="25">
+        <v>100</v>
+      </c>
+      <c r="G35" s="66">
+        <f>SUM(((G14-G12)/2),G12)</f>
+        <v>94.13</v>
+      </c>
+      <c r="H35" s="66">
+        <f>SUM(((H14-H12)/2),H12)</f>
+        <v>73.504999999999995</v>
+      </c>
+      <c r="I35" s="67">
         <f>I14+46.77</f>
         <v>149.62</v>
       </c>
-      <c r="J32" s="24">
+      <c r="J35" s="24">
         <v>50</v>
       </c>
-      <c r="K32" s="2">
-        <v>0</v>
-      </c>
-      <c r="L32" s="2">
+      <c r="K35" s="2">
+        <v>0</v>
+      </c>
+      <c r="L35" s="2">
         <v>50</v>
       </c>
-      <c r="M32" s="25">
-        <v>0</v>
-      </c>
-      <c r="N32" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="O32" s="2">
+      <c r="M35" s="25">
+        <v>0</v>
+      </c>
+      <c r="N35" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="O35" s="2">
         <v>255</v>
       </c>
-      <c r="P32" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q32" s="78"/>
-      <c r="R32" s="2"/>
-      <c r="S32" s="40"/>
-      <c r="T32" s="17" t="s">
+      <c r="P35" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q35" s="117">
+        <f>SUM(((Q14-Q12)/2),Q12)</f>
+        <v>94.13</v>
+      </c>
+      <c r="R35" s="121">
+        <f>SUM(((R14-R12)/2),R12)</f>
+        <v>-34.82</v>
+      </c>
+      <c r="S35" s="122">
+        <f>SUM(((S14-S12)/2),S12)</f>
+        <v>40.17</v>
+      </c>
+      <c r="T35" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="U32" s="65"/>
-      <c r="V32" s="24"/>
-      <c r="W32" s="25"/>
-      <c r="X32" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="Y32" s="66"/>
-      <c r="Z32" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="AA32" s="72"/>
-      <c r="AB32" s="2"/>
-      <c r="AC32" s="4"/>
-      <c r="AD32" s="118"/>
-    </row>
-    <row r="33" spans="2:35" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="113" t="s">
+      <c r="U35" s="54"/>
+      <c r="V35" s="80" t="s">
+        <v>139</v>
+      </c>
+      <c r="W35" s="144"/>
+      <c r="X35" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y35" s="59"/>
+      <c r="Z35" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA35" s="59"/>
+      <c r="AB35" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AC35" s="132"/>
+      <c r="AD35" s="86"/>
+    </row>
+    <row r="36" spans="1:30" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="87" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="114"/>
-      <c r="D33" s="113"/>
-      <c r="E33" s="119"/>
-      <c r="F33" s="119"/>
-      <c r="G33" s="119"/>
-      <c r="H33" s="119"/>
-      <c r="I33" s="119"/>
-      <c r="J33" s="119"/>
-      <c r="K33" s="119"/>
-      <c r="L33" s="119"/>
-      <c r="M33" s="119"/>
-      <c r="N33" s="119"/>
-      <c r="O33" s="119"/>
-      <c r="P33" s="119"/>
-      <c r="Q33" s="119"/>
-      <c r="R33" s="119"/>
-      <c r="S33" s="119"/>
-      <c r="T33" s="119"/>
-      <c r="U33" s="119"/>
-      <c r="V33" s="119"/>
-      <c r="W33" s="119"/>
-      <c r="X33" s="120"/>
-      <c r="Y33" s="120"/>
-      <c r="Z33" s="120"/>
-      <c r="AA33" s="120"/>
-      <c r="AB33" s="120"/>
-      <c r="AC33" s="120"/>
-      <c r="AD33" s="34"/>
-    </row>
-    <row r="34" spans="2:35" ht="17" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="95" t="s">
+      <c r="C36" s="105"/>
+      <c r="D36" s="87"/>
+      <c r="E36" s="88"/>
+      <c r="F36" s="88"/>
+      <c r="G36" s="88"/>
+      <c r="H36" s="88"/>
+      <c r="I36" s="88"/>
+      <c r="J36" s="88"/>
+      <c r="K36" s="88"/>
+      <c r="L36" s="88"/>
+      <c r="M36" s="88"/>
+      <c r="N36" s="88"/>
+      <c r="O36" s="88"/>
+      <c r="P36" s="88"/>
+      <c r="Q36" s="88"/>
+      <c r="R36" s="88"/>
+      <c r="S36" s="88"/>
+      <c r="T36" s="88"/>
+      <c r="U36" s="88"/>
+      <c r="V36" s="88"/>
+      <c r="W36" s="88"/>
+      <c r="X36" s="89"/>
+      <c r="Y36" s="89"/>
+      <c r="Z36" s="89"/>
+      <c r="AA36" s="89"/>
+      <c r="AB36" s="89"/>
+      <c r="AC36" s="89"/>
+      <c r="AD36" s="34"/>
+    </row>
+    <row r="37" spans="1:30" ht="17" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="96"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="39"/>
-      <c r="K34" s="31"/>
-      <c r="L34" s="31"/>
-      <c r="M34" s="35"/>
-      <c r="N34" s="39"/>
-      <c r="O34" s="31"/>
-      <c r="P34" s="35"/>
-      <c r="Q34" s="39"/>
-      <c r="R34" s="31"/>
-      <c r="S34" s="41"/>
-      <c r="T34" s="2"/>
-      <c r="U34" s="25"/>
-      <c r="V34" s="24"/>
-      <c r="W34" s="25"/>
-      <c r="X34" s="36"/>
-      <c r="Y34" s="38"/>
-      <c r="Z34" s="37"/>
-      <c r="AA34" s="38"/>
-      <c r="AB34" s="37"/>
-      <c r="AC34" s="38"/>
-      <c r="AD34" s="118" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="35" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B35" s="95" t="s">
-        <v>45</v>
-      </c>
-      <c r="C35" s="96"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="24"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="25"/>
-      <c r="N35" s="24"/>
-      <c r="O35" s="2"/>
-      <c r="P35" s="25"/>
-      <c r="Q35" s="24"/>
-      <c r="R35" s="2"/>
-      <c r="S35" s="40"/>
-      <c r="T35" s="2"/>
-      <c r="U35" s="25"/>
-      <c r="V35" s="24"/>
-      <c r="W35" s="25"/>
-      <c r="X35" s="32"/>
-      <c r="Y35" s="4"/>
-      <c r="Z35" s="3"/>
-      <c r="AA35" s="4"/>
-      <c r="AB35" s="3"/>
-      <c r="AC35" s="4"/>
-      <c r="AD35" s="118"/>
-    </row>
-    <row r="36" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B36" s="95" t="s">
-        <v>46</v>
-      </c>
-      <c r="C36" s="96"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="24"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="25"/>
-      <c r="N36" s="24"/>
-      <c r="O36" s="2"/>
-      <c r="P36" s="25"/>
-      <c r="Q36" s="24"/>
-      <c r="R36" s="2"/>
-      <c r="S36" s="40"/>
-      <c r="T36" s="2"/>
-      <c r="U36" s="25"/>
-      <c r="V36" s="24"/>
-      <c r="W36" s="25"/>
-      <c r="X36" s="32"/>
-      <c r="Y36" s="4"/>
-      <c r="Z36" s="3"/>
-      <c r="AA36" s="4"/>
-      <c r="AB36" s="3"/>
-      <c r="AC36" s="4"/>
-      <c r="AD36" s="118"/>
-    </row>
-    <row r="37" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B37" s="95" t="s">
-        <v>47</v>
-      </c>
-      <c r="C37" s="96"/>
+      <c r="C37" s="104"/>
       <c r="D37" s="24"/>
       <c r="E37" s="2"/>
       <c r="F37" s="25"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="25"/>
-      <c r="J37" s="24"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="25"/>
-      <c r="N37" s="24"/>
-      <c r="O37" s="2"/>
-      <c r="P37" s="25"/>
-      <c r="Q37" s="24"/>
-      <c r="R37" s="2"/>
-      <c r="S37" s="40"/>
+      <c r="J37" s="39"/>
+      <c r="K37" s="31"/>
+      <c r="L37" s="31"/>
+      <c r="M37" s="35"/>
+      <c r="N37" s="39"/>
+      <c r="O37" s="31"/>
+      <c r="P37" s="35"/>
+      <c r="Q37" s="39"/>
+      <c r="R37" s="31"/>
+      <c r="S37" s="41"/>
       <c r="T37" s="2"/>
       <c r="U37" s="25"/>
       <c r="V37" s="24"/>
       <c r="W37" s="25"/>
-      <c r="X37" s="32"/>
-      <c r="Y37" s="4"/>
-      <c r="Z37" s="3"/>
-      <c r="AA37" s="4"/>
-      <c r="AB37" s="3"/>
-      <c r="AC37" s="4"/>
-      <c r="AD37" s="118"/>
-    </row>
-    <row r="38" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B38" s="95" t="s">
-        <v>48</v>
-      </c>
-      <c r="C38" s="96"/>
+      <c r="X37" s="36"/>
+      <c r="Y37" s="38"/>
+      <c r="Z37" s="37"/>
+      <c r="AA37" s="38"/>
+      <c r="AB37" s="37"/>
+      <c r="AC37" s="38"/>
+      <c r="AD37" s="86" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="B38" s="103" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="104"/>
       <c r="D38" s="24"/>
       <c r="E38" s="2"/>
       <c r="F38" s="25"/>
@@ -3667,13 +4177,13 @@
       <c r="AA38" s="4"/>
       <c r="AB38" s="3"/>
       <c r="AC38" s="4"/>
-      <c r="AD38" s="118"/>
-    </row>
-    <row r="39" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B39" s="95" t="s">
-        <v>49</v>
-      </c>
-      <c r="C39" s="96"/>
+      <c r="AD38" s="86"/>
+    </row>
+    <row r="39" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="B39" s="103" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="104"/>
       <c r="D39" s="24"/>
       <c r="E39" s="2"/>
       <c r="F39" s="25"/>
@@ -3700,13 +4210,13 @@
       <c r="AA39" s="4"/>
       <c r="AB39" s="3"/>
       <c r="AC39" s="4"/>
-      <c r="AD39" s="118"/>
-    </row>
-    <row r="40" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B40" s="95" t="s">
-        <v>50</v>
-      </c>
-      <c r="C40" s="96"/>
+      <c r="AD39" s="86"/>
+    </row>
+    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="B40" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="104"/>
       <c r="D40" s="24"/>
       <c r="E40" s="2"/>
       <c r="F40" s="25"/>
@@ -3733,13 +4243,13 @@
       <c r="AA40" s="4"/>
       <c r="AB40" s="3"/>
       <c r="AC40" s="4"/>
-      <c r="AD40" s="118"/>
-    </row>
-    <row r="41" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B41" s="95" t="s">
-        <v>51</v>
-      </c>
-      <c r="C41" s="96"/>
+      <c r="AD40" s="86"/>
+    </row>
+    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="B41" s="103" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" s="104"/>
       <c r="D41" s="24"/>
       <c r="E41" s="2"/>
       <c r="F41" s="25"/>
@@ -3766,13 +4276,13 @@
       <c r="AA41" s="4"/>
       <c r="AB41" s="3"/>
       <c r="AC41" s="4"/>
-      <c r="AD41" s="118"/>
-    </row>
-    <row r="42" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B42" s="95" t="s">
-        <v>52</v>
-      </c>
-      <c r="C42" s="96"/>
+      <c r="AD41" s="86"/>
+    </row>
+    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="B42" s="103" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="104"/>
       <c r="D42" s="24"/>
       <c r="E42" s="2"/>
       <c r="F42" s="25"/>
@@ -3799,13 +4309,13 @@
       <c r="AA42" s="4"/>
       <c r="AB42" s="3"/>
       <c r="AC42" s="4"/>
-      <c r="AD42" s="118"/>
-    </row>
-    <row r="43" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B43" s="95" t="s">
-        <v>53</v>
-      </c>
-      <c r="C43" s="96"/>
+      <c r="AD42" s="86"/>
+    </row>
+    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="B43" s="103" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" s="104"/>
       <c r="D43" s="24"/>
       <c r="E43" s="2"/>
       <c r="F43" s="25"/>
@@ -3832,13 +4342,13 @@
       <c r="AA43" s="4"/>
       <c r="AB43" s="3"/>
       <c r="AC43" s="4"/>
-      <c r="AD43" s="118"/>
-    </row>
-    <row r="44" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B44" s="95" t="s">
-        <v>54</v>
-      </c>
-      <c r="C44" s="96"/>
+      <c r="AD43" s="86"/>
+    </row>
+    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="B44" s="103" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" s="104"/>
       <c r="D44" s="24"/>
       <c r="E44" s="2"/>
       <c r="F44" s="25"/>
@@ -3865,13 +4375,13 @@
       <c r="AA44" s="4"/>
       <c r="AB44" s="3"/>
       <c r="AC44" s="4"/>
-      <c r="AD44" s="118"/>
-    </row>
-    <row r="45" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B45" s="95" t="s">
-        <v>55</v>
-      </c>
-      <c r="C45" s="96"/>
+      <c r="AD44" s="86"/>
+    </row>
+    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="B45" s="103" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="104"/>
       <c r="D45" s="24"/>
       <c r="E45" s="2"/>
       <c r="F45" s="25"/>
@@ -3898,13 +4408,13 @@
       <c r="AA45" s="4"/>
       <c r="AB45" s="3"/>
       <c r="AC45" s="4"/>
-      <c r="AD45" s="118"/>
-    </row>
-    <row r="46" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B46" s="95" t="s">
-        <v>56</v>
-      </c>
-      <c r="C46" s="96"/>
+      <c r="AD45" s="86"/>
+    </row>
+    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="B46" s="103" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" s="104"/>
       <c r="D46" s="24"/>
       <c r="E46" s="2"/>
       <c r="F46" s="25"/>
@@ -3931,13 +4441,13 @@
       <c r="AA46" s="4"/>
       <c r="AB46" s="3"/>
       <c r="AC46" s="4"/>
-      <c r="AD46" s="118"/>
-    </row>
-    <row r="47" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B47" s="95" t="s">
-        <v>57</v>
-      </c>
-      <c r="C47" s="96"/>
+      <c r="AD46" s="86"/>
+    </row>
+    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="B47" s="103" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" s="104"/>
       <c r="D47" s="24"/>
       <c r="E47" s="2"/>
       <c r="F47" s="25"/>
@@ -3964,13 +4474,13 @@
       <c r="AA47" s="4"/>
       <c r="AB47" s="3"/>
       <c r="AC47" s="4"/>
-      <c r="AD47" s="118"/>
-    </row>
-    <row r="48" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B48" s="95" t="s">
-        <v>58</v>
-      </c>
-      <c r="C48" s="96"/>
+      <c r="AD47" s="86"/>
+    </row>
+    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="B48" s="103" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" s="104"/>
       <c r="D48" s="24"/>
       <c r="E48" s="2"/>
       <c r="F48" s="25"/>
@@ -3997,17 +4507,13 @@
       <c r="AA48" s="4"/>
       <c r="AB48" s="3"/>
       <c r="AC48" s="4"/>
-      <c r="AD48" s="118"/>
-      <c r="AH48" s="99" t="s">
-        <v>130</v>
-      </c>
-      <c r="AI48" s="99"/>
-    </row>
-    <row r="49" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="B49" s="95" t="s">
-        <v>59</v>
-      </c>
-      <c r="C49" s="96"/>
+      <c r="AD48" s="86"/>
+    </row>
+    <row r="49" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B49" s="103" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" s="104"/>
       <c r="D49" s="24"/>
       <c r="E49" s="2"/>
       <c r="F49" s="25"/>
@@ -4034,13 +4540,13 @@
       <c r="AA49" s="4"/>
       <c r="AB49" s="3"/>
       <c r="AC49" s="4"/>
-      <c r="AD49" s="118"/>
-    </row>
-    <row r="50" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="B50" s="95" t="s">
-        <v>60</v>
-      </c>
-      <c r="C50" s="96"/>
+      <c r="AD49" s="86"/>
+    </row>
+    <row r="50" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B50" s="103" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" s="104"/>
       <c r="D50" s="24"/>
       <c r="E50" s="2"/>
       <c r="F50" s="25"/>
@@ -4067,13 +4573,13 @@
       <c r="AA50" s="4"/>
       <c r="AB50" s="3"/>
       <c r="AC50" s="4"/>
-      <c r="AD50" s="118"/>
-    </row>
-    <row r="51" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="B51" s="95" t="s">
-        <v>61</v>
-      </c>
-      <c r="C51" s="96"/>
+      <c r="AD50" s="86"/>
+    </row>
+    <row r="51" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B51" s="103" t="s">
+        <v>58</v>
+      </c>
+      <c r="C51" s="104"/>
       <c r="D51" s="24"/>
       <c r="E51" s="2"/>
       <c r="F51" s="25"/>
@@ -4100,13 +4606,17 @@
       <c r="AA51" s="4"/>
       <c r="AB51" s="3"/>
       <c r="AC51" s="4"/>
-      <c r="AD51" s="118"/>
-    </row>
-    <row r="52" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="B52" s="95" t="s">
-        <v>62</v>
-      </c>
-      <c r="C52" s="96"/>
+      <c r="AD51" s="86"/>
+      <c r="AH51" s="82" t="s">
+        <v>105</v>
+      </c>
+      <c r="AI51" s="82"/>
+    </row>
+    <row r="52" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B52" s="103" t="s">
+        <v>59</v>
+      </c>
+      <c r="C52" s="104"/>
       <c r="D52" s="24"/>
       <c r="E52" s="2"/>
       <c r="F52" s="25"/>
@@ -4133,76 +4643,187 @@
       <c r="AA52" s="4"/>
       <c r="AB52" s="3"/>
       <c r="AC52" s="4"/>
-      <c r="AD52" s="118"/>
-    </row>
-    <row r="53" spans="2:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="97" t="s">
+      <c r="AD52" s="86"/>
+    </row>
+    <row r="53" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B53" s="103" t="s">
+        <v>60</v>
+      </c>
+      <c r="C53" s="104"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="25"/>
+      <c r="J53" s="24"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="25"/>
+      <c r="N53" s="24"/>
+      <c r="O53" s="2"/>
+      <c r="P53" s="25"/>
+      <c r="Q53" s="24"/>
+      <c r="R53" s="2"/>
+      <c r="S53" s="40"/>
+      <c r="T53" s="2"/>
+      <c r="U53" s="25"/>
+      <c r="V53" s="24"/>
+      <c r="W53" s="25"/>
+      <c r="X53" s="32"/>
+      <c r="Y53" s="4"/>
+      <c r="Z53" s="3"/>
+      <c r="AA53" s="4"/>
+      <c r="AB53" s="3"/>
+      <c r="AC53" s="4"/>
+      <c r="AD53" s="86"/>
+    </row>
+    <row r="54" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B54" s="103" t="s">
+        <v>61</v>
+      </c>
+      <c r="C54" s="104"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="25"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="25"/>
+      <c r="J54" s="24"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="25"/>
+      <c r="N54" s="24"/>
+      <c r="O54" s="2"/>
+      <c r="P54" s="25"/>
+      <c r="Q54" s="24"/>
+      <c r="R54" s="2"/>
+      <c r="S54" s="40"/>
+      <c r="T54" s="2"/>
+      <c r="U54" s="25"/>
+      <c r="V54" s="24"/>
+      <c r="W54" s="25"/>
+      <c r="X54" s="32"/>
+      <c r="Y54" s="4"/>
+      <c r="Z54" s="3"/>
+      <c r="AA54" s="4"/>
+      <c r="AB54" s="3"/>
+      <c r="AC54" s="4"/>
+      <c r="AD54" s="86"/>
+    </row>
+    <row r="55" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B55" s="103" t="s">
+        <v>62</v>
+      </c>
+      <c r="C55" s="104"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="25"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="25"/>
+      <c r="J55" s="24"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+      <c r="M55" s="25"/>
+      <c r="N55" s="24"/>
+      <c r="O55" s="2"/>
+      <c r="P55" s="25"/>
+      <c r="Q55" s="24"/>
+      <c r="R55" s="2"/>
+      <c r="S55" s="40"/>
+      <c r="T55" s="2"/>
+      <c r="U55" s="25"/>
+      <c r="V55" s="24"/>
+      <c r="W55" s="25"/>
+      <c r="X55" s="32"/>
+      <c r="Y55" s="4"/>
+      <c r="Z55" s="3"/>
+      <c r="AA55" s="4"/>
+      <c r="AB55" s="3"/>
+      <c r="AC55" s="4"/>
+      <c r="AD55" s="86"/>
+    </row>
+    <row r="56" spans="2:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="106" t="s">
         <v>63</v>
       </c>
-      <c r="C53" s="98"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="30"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
-      <c r="I53" s="30"/>
-      <c r="J53" s="29"/>
-      <c r="K53" s="5"/>
-      <c r="L53" s="5"/>
-      <c r="M53" s="30"/>
-      <c r="N53" s="29"/>
-      <c r="O53" s="5"/>
-      <c r="P53" s="30"/>
-      <c r="Q53" s="29"/>
-      <c r="R53" s="5"/>
-      <c r="S53" s="42"/>
-      <c r="T53" s="5"/>
-      <c r="U53" s="30"/>
-      <c r="V53" s="29"/>
-      <c r="W53" s="30"/>
-      <c r="X53" s="33"/>
-      <c r="Y53" s="7"/>
-      <c r="Z53" s="6"/>
-      <c r="AA53" s="7"/>
-      <c r="AB53" s="6"/>
-      <c r="AC53" s="7"/>
-      <c r="AD53" s="118"/>
+      <c r="C56" s="107"/>
+      <c r="D56" s="29"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="30"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="30"/>
+      <c r="J56" s="29"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="5"/>
+      <c r="M56" s="30"/>
+      <c r="N56" s="29"/>
+      <c r="O56" s="5"/>
+      <c r="P56" s="30"/>
+      <c r="Q56" s="29"/>
+      <c r="R56" s="5"/>
+      <c r="S56" s="42"/>
+      <c r="T56" s="5"/>
+      <c r="U56" s="30"/>
+      <c r="V56" s="29"/>
+      <c r="W56" s="30"/>
+      <c r="X56" s="33"/>
+      <c r="Y56" s="7"/>
+      <c r="Z56" s="6"/>
+      <c r="AA56" s="7"/>
+      <c r="AB56" s="6"/>
+      <c r="AC56" s="7"/>
+      <c r="AD56" s="86"/>
     </row>
   </sheetData>
-  <mergeCells count="61">
-    <mergeCell ref="AH28:AI28"/>
-    <mergeCell ref="AH48:AI48"/>
-    <mergeCell ref="T16:AC16"/>
-    <mergeCell ref="AD18:AD32"/>
-    <mergeCell ref="D33:AC33"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="T17:U17"/>
-    <mergeCell ref="V17:W17"/>
-    <mergeCell ref="X17:Y17"/>
-    <mergeCell ref="Z17:AA17"/>
-    <mergeCell ref="AB17:AC17"/>
-    <mergeCell ref="AD34:AD53"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
+  <mergeCells count="88">
+    <mergeCell ref="Z34:AA34"/>
+    <mergeCell ref="AB34:AC34"/>
+    <mergeCell ref="J34:M34"/>
+    <mergeCell ref="N34:P34"/>
+    <mergeCell ref="Q34:S34"/>
+    <mergeCell ref="V34:W34"/>
+    <mergeCell ref="X34:Y34"/>
+    <mergeCell ref="B33:C34"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="X22:Y22"/>
+    <mergeCell ref="Z22:AA22"/>
+    <mergeCell ref="AB22:AC22"/>
+    <mergeCell ref="B28:C29"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="J29:M29"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="Q29:S29"/>
+    <mergeCell ref="V29:W29"/>
+    <mergeCell ref="X29:Y29"/>
+    <mergeCell ref="Z29:AA29"/>
+    <mergeCell ref="AB29:AC29"/>
+    <mergeCell ref="B21:C22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="N22:P22"/>
+    <mergeCell ref="Q22:S22"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B56:C56"/>
     <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B50:C50"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="D16:F16"/>
@@ -4213,27 +4834,46 @@
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B50:C50"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
     <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="AH30:AI30"/>
+    <mergeCell ref="AH51:AI51"/>
+    <mergeCell ref="T16:AC16"/>
+    <mergeCell ref="AD18:AD35"/>
+    <mergeCell ref="D36:AC36"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="V17:W17"/>
+    <mergeCell ref="X17:Y17"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="AD37:AD56"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="V22:W22"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="R25:R26" formula="1"/>
+  </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>